<commit_message>
ADDING SUMMARY SHEET 2
</commit_message>
<xml_diff>
--- a/Linux_2k_clean_analysis.xlsx
+++ b/Linux_2k_clean_analysis.xlsx
@@ -12563,7 +12563,7 @@
       </c>
       <c r="B607" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C607" t="n">
@@ -12571,7 +12571,7 @@
       </c>
       <c r="D607" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jun 15 04:06:18", "HOSTNAME": "combo", "PID": "21416", "USERNAME": "cyrus", "UID": "0"}</t>
+          <t>{"TIMESTAMP": "Jun 15 04:06:18", "HOSTNAME": "combo", "PID": "21416", "STATE": "opened", "USERNAME": "cyrus", "UID": "0"}</t>
         </is>
       </c>
     </row>
@@ -12583,7 +12583,7 @@
       </c>
       <c r="B608" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C608" t="n">
@@ -12591,7 +12591,7 @@
       </c>
       <c r="D608" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul 27 04:21:39", "HOSTNAME": "combo", "PID": "31373", "USERNAME": "news", "UID": "0"}</t>
+          <t>{"TIMESTAMP": "Jul 27 04:21:39", "HOSTNAME": "combo", "PID": "31373", "STATE": "opened", "USERNAME": "news", "UID": "0"}</t>
         </is>
       </c>
     </row>
@@ -12603,7 +12603,7 @@
       </c>
       <c r="B609" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C609" t="n">
@@ -12611,7 +12611,7 @@
       </c>
       <c r="D609" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jun 15 04:12:42", "HOSTNAME": "combo", "PID": "22644", "USERNAME": "news", "UID": "0"}</t>
+          <t>{"TIMESTAMP": "Jun 15 04:12:42", "HOSTNAME": "combo", "PID": "22644", "STATE": "opened", "USERNAME": "news", "UID": "0"}</t>
         </is>
       </c>
     </row>
@@ -12623,7 +12623,7 @@
       </c>
       <c r="B610" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C610" t="n">
@@ -12631,7 +12631,7 @@
       </c>
       <c r="D610" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul 27 04:16:07", "HOSTNAME": "combo", "PID": "30999", "USERNAME": "cyrus", "UID": "0"}</t>
+          <t>{"TIMESTAMP": "Jul 27 04:16:07", "HOSTNAME": "combo", "PID": "30999", "STATE": "opened", "USERNAME": "cyrus", "UID": "0"}</t>
         </is>
       </c>
     </row>
@@ -12643,7 +12643,7 @@
       </c>
       <c r="B611" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C611" t="n">
@@ -12651,7 +12651,7 @@
       </c>
       <c r="D611" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul 18 04:03:24", "HOSTNAME": "combo", "PID": "26046", "USERNAME": "cyrus", "UID": "0"}</t>
+          <t>{"TIMESTAMP": "Jul 18 04:03:24", "HOSTNAME": "combo", "PID": "26046", "STATE": "opened", "USERNAME": "cyrus", "UID": "0"}</t>
         </is>
       </c>
     </row>
@@ -12663,7 +12663,7 @@
       </c>
       <c r="B612" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C612" t="n">
@@ -12671,7 +12671,7 @@
       </c>
       <c r="D612" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul 18 04:09:29", "HOSTNAME": "combo", "PID": "27272", "USERNAME": "news", "UID": "0"}</t>
+          <t>{"TIMESTAMP": "Jul 18 04:09:29", "HOSTNAME": "combo", "PID": "27272", "STATE": "opened", "USERNAME": "news", "UID": "0"}</t>
         </is>
       </c>
     </row>
@@ -12683,7 +12683,7 @@
       </c>
       <c r="B613" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C613" t="n">
@@ -12691,7 +12691,7 @@
       </c>
       <c r="D613" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jun 24 04:05:34", "HOSTNAME": "combo", "PID": "26938", "USERNAME": "cyrus", "UID": "0"}</t>
+          <t>{"TIMESTAMP": "Jun 24 04:05:34", "HOSTNAME": "combo", "PID": "26938", "STATE": "opened", "USERNAME": "cyrus", "UID": "0"}</t>
         </is>
       </c>
     </row>
@@ -12703,7 +12703,7 @@
       </c>
       <c r="B614" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C614" t="n">
@@ -12711,7 +12711,7 @@
       </c>
       <c r="D614" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jun 24 04:11:12", "HOSTNAME": "combo", "PID": "27311", "USERNAME": "news", "UID": "0"}</t>
+          <t>{"TIMESTAMP": "Jun 24 04:11:12", "HOSTNAME": "combo", "PID": "27311", "STATE": "opened", "USERNAME": "news", "UID": "0"}</t>
         </is>
       </c>
     </row>
@@ -12723,7 +12723,7 @@
       </c>
       <c r="B615" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C615" t="n">
@@ -12731,7 +12731,7 @@
       </c>
       <c r="D615" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jun 25 04:04:25", "HOSTNAME": "combo", "PID": "29690", "USERNAME": "cyrus", "UID": "0"}</t>
+          <t>{"TIMESTAMP": "Jun 25 04:04:25", "HOSTNAME": "combo", "PID": "29690", "STATE": "opened", "USERNAME": "cyrus", "UID": "0"}</t>
         </is>
       </c>
     </row>
@@ -12743,7 +12743,7 @@
       </c>
       <c r="B616" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C616" t="n">
@@ -12751,7 +12751,7 @@
       </c>
       <c r="D616" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jun 25 04:10:34", "HOSTNAME": "combo", "PID": "30934", "USERNAME": "news", "UID": "0"}</t>
+          <t>{"TIMESTAMP": "Jun 25 04:10:34", "HOSTNAME": "combo", "PID": "30934", "STATE": "opened", "USERNAME": "news", "UID": "0"}</t>
         </is>
       </c>
     </row>
@@ -12763,7 +12763,7 @@
       </c>
       <c r="B617" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C617" t="n">
@@ -12771,7 +12771,7 @@
       </c>
       <c r="D617" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul  3 04:14:00", "HOSTNAME": "combo", "PID": "28416", "USERNAME": "news", "UID": "0"}</t>
+          <t>{"TIMESTAMP": "Jul  3 04:14:00", "HOSTNAME": "combo", "PID": "28416", "STATE": "opened", "USERNAME": "news", "UID": "0"}</t>
         </is>
       </c>
     </row>
@@ -12783,7 +12783,7 @@
       </c>
       <c r="B618" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C618" t="n">
@@ -12791,7 +12791,7 @@
       </c>
       <c r="D618" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul 17 04:08:08", "HOSTNAME": "combo", "PID": "19686", "USERNAME": "cyrus", "UID": "0"}</t>
+          <t>{"TIMESTAMP": "Jul 17 04:08:08", "HOSTNAME": "combo", "PID": "19686", "STATE": "opened", "USERNAME": "cyrus", "UID": "0"}</t>
         </is>
       </c>
     </row>
@@ -12803,7 +12803,7 @@
       </c>
       <c r="B619" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C619" t="n">
@@ -12811,7 +12811,7 @@
       </c>
       <c r="D619" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul 17 04:13:57", "HOSTNAME": "combo", "PID": "20282", "USERNAME": "news", "UID": "0"}</t>
+          <t>{"TIMESTAMP": "Jul 17 04:13:57", "HOSTNAME": "combo", "PID": "20282", "STATE": "opened", "USERNAME": "news", "UID": "0"}</t>
         </is>
       </c>
     </row>
@@ -12823,7 +12823,7 @@
       </c>
       <c r="B620" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C620" t="n">
@@ -12831,7 +12831,7 @@
       </c>
       <c r="D620" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jun 23 04:05:28", "HOSTNAME": "combo", "PID": "19534", "USERNAME": "cyrus", "UID": "0"}</t>
+          <t>{"TIMESTAMP": "Jun 23 04:05:28", "HOSTNAME": "combo", "PID": "19534", "STATE": "opened", "USERNAME": "cyrus", "UID": "0"}</t>
         </is>
       </c>
     </row>
@@ -12843,7 +12843,7 @@
       </c>
       <c r="B621" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C621" t="n">
@@ -12851,7 +12851,7 @@
       </c>
       <c r="D621" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jun 23 04:13:08", "HOSTNAME": "combo", "PID": "24180", "USERNAME": "news", "UID": "0"}</t>
+          <t>{"TIMESTAMP": "Jun 23 04:13:08", "HOSTNAME": "combo", "PID": "24180", "STATE": "opened", "USERNAME": "news", "UID": "0"}</t>
         </is>
       </c>
     </row>
@@ -12863,7 +12863,7 @@
       </c>
       <c r="B622" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C622" t="n">
@@ -12871,7 +12871,7 @@
       </c>
       <c r="D622" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul 13 04:10:41", "HOSTNAME": "combo", "PID": "6863", "USERNAME": "news", "UID": "0"}</t>
+          <t>{"TIMESTAMP": "Jul 13 04:10:41", "HOSTNAME": "combo", "PID": "6863", "STATE": "opened", "USERNAME": "news", "UID": "0"}</t>
         </is>
       </c>
     </row>
@@ -12883,7 +12883,7 @@
       </c>
       <c r="B623" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C623" t="n">
@@ -12891,7 +12891,7 @@
       </c>
       <c r="D623" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul 14 04:08:24", "HOSTNAME": "combo", "PID": "9355", "USERNAME": "cyrus", "UID": "0"}</t>
+          <t>{"TIMESTAMP": "Jul 14 04:08:24", "HOSTNAME": "combo", "PID": "9355", "STATE": "opened", "USERNAME": "cyrus", "UID": "0"}</t>
         </is>
       </c>
     </row>
@@ -12903,7 +12903,7 @@
       </c>
       <c r="B624" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C624" t="n">
@@ -12911,7 +12911,7 @@
       </c>
       <c r="D624" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul 14 04:14:38", "HOSTNAME": "combo", "PID": "10583", "USERNAME": "news", "UID": "0"}</t>
+          <t>{"TIMESTAMP": "Jul 14 04:14:38", "HOSTNAME": "combo", "PID": "10583", "STATE": "opened", "USERNAME": "news", "UID": "0"}</t>
         </is>
       </c>
     </row>
@@ -12923,7 +12923,7 @@
       </c>
       <c r="B625" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C625" t="n">
@@ -12931,7 +12931,7 @@
       </c>
       <c r="D625" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul 15 04:05:02", "HOSTNAME": "combo", "PID": "13238", "USERNAME": "cyrus", "UID": "0"}</t>
+          <t>{"TIMESTAMP": "Jul 15 04:05:02", "HOSTNAME": "combo", "PID": "13238", "STATE": "opened", "USERNAME": "cyrus", "UID": "0"}</t>
         </is>
       </c>
     </row>
@@ -12943,7 +12943,7 @@
       </c>
       <c r="B626" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C626" t="n">
@@ -12951,7 +12951,7 @@
       </c>
       <c r="D626" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul 15 04:10:45", "HOSTNAME": "combo", "PID": "13611", "USERNAME": "news", "UID": "0"}</t>
+          <t>{"TIMESTAMP": "Jul 15 04:10:45", "HOSTNAME": "combo", "PID": "13611", "STATE": "opened", "USERNAME": "news", "UID": "0"}</t>
         </is>
       </c>
     </row>
@@ -12963,7 +12963,7 @@
       </c>
       <c r="B627" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C627" t="n">
@@ -12971,7 +12971,7 @@
       </c>
       <c r="D627" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul 16 04:07:32", "HOSTNAME": "combo", "PID": "16058", "USERNAME": "cyrus", "UID": "0"}</t>
+          <t>{"TIMESTAMP": "Jul 16 04:07:32", "HOSTNAME": "combo", "PID": "16058", "STATE": "opened", "USERNAME": "cyrus", "UID": "0"}</t>
         </is>
       </c>
     </row>
@@ -12983,7 +12983,7 @@
       </c>
       <c r="B628" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C628" t="n">
@@ -12991,7 +12991,7 @@
       </c>
       <c r="D628" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul 16 04:13:59", "HOSTNAME": "combo", "PID": "17286", "USERNAME": "news", "UID": "0"}</t>
+          <t>{"TIMESTAMP": "Jul 16 04:13:59", "HOSTNAME": "combo", "PID": "17286", "STATE": "opened", "USERNAME": "news", "UID": "0"}</t>
         </is>
       </c>
     </row>
@@ -13003,7 +13003,7 @@
       </c>
       <c r="B629" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C629" t="n">
@@ -13011,7 +13011,7 @@
       </c>
       <c r="D629" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jun 28 04:03:15", "HOSTNAME": "combo", "PID": "10735", "USERNAME": "cyrus", "UID": "0"}</t>
+          <t>{"TIMESTAMP": "Jun 28 04:03:15", "HOSTNAME": "combo", "PID": "10735", "STATE": "opened", "USERNAME": "cyrus", "UID": "0"}</t>
         </is>
       </c>
     </row>
@@ -13023,7 +13023,7 @@
       </c>
       <c r="B630" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C630" t="n">
@@ -13031,7 +13031,7 @@
       </c>
       <c r="D630" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jun 28 04:09:00", "HOSTNAME": "combo", "PID": "11106", "USERNAME": "news", "UID": "0"}</t>
+          <t>{"TIMESTAMP": "Jun 28 04:09:00", "HOSTNAME": "combo", "PID": "11106", "STATE": "opened", "USERNAME": "news", "UID": "0"}</t>
         </is>
       </c>
     </row>
@@ -13043,7 +13043,7 @@
       </c>
       <c r="B631" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C631" t="n">
@@ -13051,7 +13051,7 @@
       </c>
       <c r="D631" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jun 26 04:04:17", "HOSTNAME": "combo", "PID": "945", "USERNAME": "cyrus", "UID": "0"}</t>
+          <t>{"TIMESTAMP": "Jun 26 04:04:17", "HOSTNAME": "combo", "PID": "945", "STATE": "opened", "USERNAME": "cyrus", "UID": "0"}</t>
         </is>
       </c>
     </row>
@@ -13063,7 +13063,7 @@
       </c>
       <c r="B632" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C632" t="n">
@@ -13071,7 +13071,7 @@
       </c>
       <c r="D632" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jun 26 04:10:02", "HOSTNAME": "combo", "PID": "1546", "USERNAME": "news", "UID": "0"}</t>
+          <t>{"TIMESTAMP": "Jun 26 04:10:02", "HOSTNAME": "combo", "PID": "1546", "STATE": "opened", "USERNAME": "news", "UID": "0"}</t>
         </is>
       </c>
     </row>
@@ -13083,7 +13083,7 @@
       </c>
       <c r="B633" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C633" t="n">
@@ -13091,7 +13091,7 @@
       </c>
       <c r="D633" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jun 27 04:02:47", "HOSTNAME": "combo", "PID": "7031", "USERNAME": "cyrus", "UID": "0"}</t>
+          <t>{"TIMESTAMP": "Jun 27 04:02:47", "HOSTNAME": "combo", "PID": "7031", "STATE": "opened", "USERNAME": "cyrus", "UID": "0"}</t>
         </is>
       </c>
     </row>
@@ -13103,7 +13103,7 @@
       </c>
       <c r="B634" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C634" t="n">
@@ -13111,7 +13111,7 @@
       </c>
       <c r="D634" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jun 27 04:08:56", "HOSTNAME": "combo", "PID": "8269", "USERNAME": "news", "UID": "0"}</t>
+          <t>{"TIMESTAMP": "Jun 27 04:08:56", "HOSTNAME": "combo", "PID": "8269", "STATE": "opened", "USERNAME": "news", "UID": "0"}</t>
         </is>
       </c>
     </row>
@@ -13123,7 +13123,7 @@
       </c>
       <c r="B635" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C635" t="n">
@@ -13131,7 +13131,7 @@
       </c>
       <c r="D635" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul 12 04:03:40", "HOSTNAME": "combo", "PID": "2605", "USERNAME": "cyrus", "UID": "0"}</t>
+          <t>{"TIMESTAMP": "Jul 12 04:03:40", "HOSTNAME": "combo", "PID": "2605", "STATE": "opened", "USERNAME": "cyrus", "UID": "0"}</t>
         </is>
       </c>
     </row>
@@ -13143,7 +13143,7 @@
       </c>
       <c r="B636" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C636" t="n">
@@ -13151,7 +13151,7 @@
       </c>
       <c r="D636" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul 12 04:09:49", "HOSTNAME": "combo", "PID": "3833", "USERNAME": "news", "UID": "0"}</t>
+          <t>{"TIMESTAMP": "Jul 12 04:09:49", "HOSTNAME": "combo", "PID": "3833", "STATE": "opened", "USERNAME": "news", "UID": "0"}</t>
         </is>
       </c>
     </row>
@@ -13163,7 +13163,7 @@
       </c>
       <c r="B637" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C637" t="n">
@@ -13171,7 +13171,7 @@
       </c>
       <c r="D637" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul 13 04:04:44", "HOSTNAME": "combo", "PID": "6486", "USERNAME": "cyrus", "UID": "0"}</t>
+          <t>{"TIMESTAMP": "Jul 13 04:04:44", "HOSTNAME": "combo", "PID": "6486", "STATE": "opened", "USERNAME": "cyrus", "UID": "0"}</t>
         </is>
       </c>
     </row>
@@ -13183,7 +13183,7 @@
       </c>
       <c r="B638" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C638" t="n">
@@ -13191,7 +13191,7 @@
       </c>
       <c r="D638" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul 11 04:03:03", "HOSTNAME": "combo", "PID": "32237", "USERNAME": "cyrus", "UID": "0"}</t>
+          <t>{"TIMESTAMP": "Jul 11 04:03:03", "HOSTNAME": "combo", "PID": "32237", "STATE": "opened", "USERNAME": "cyrus", "UID": "0"}</t>
         </is>
       </c>
     </row>
@@ -13203,7 +13203,7 @@
       </c>
       <c r="B639" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C639" t="n">
@@ -13211,7 +13211,7 @@
       </c>
       <c r="D639" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul 11 04:08:37", "HOSTNAME": "combo", "PID": "32608", "USERNAME": "news", "UID": "0"}</t>
+          <t>{"TIMESTAMP": "Jul 11 04:08:37", "HOSTNAME": "combo", "PID": "32608", "STATE": "opened", "USERNAME": "news", "UID": "0"}</t>
         </is>
       </c>
     </row>
@@ -13223,7 +13223,7 @@
       </c>
       <c r="B640" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C640" t="n">
@@ -13231,7 +13231,7 @@
       </c>
       <c r="D640" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jun 22 04:11:42", "HOSTNAME": "combo", "PID": "17037", "USERNAME": "news", "UID": "0"}</t>
+          <t>{"TIMESTAMP": "Jun 22 04:11:42", "HOSTNAME": "combo", "PID": "17037", "STATE": "opened", "USERNAME": "news", "UID": "0"}</t>
         </is>
       </c>
     </row>
@@ -13243,7 +13243,7 @@
       </c>
       <c r="B641" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C641" t="n">
@@ -13251,7 +13251,7 @@
       </c>
       <c r="D641" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jun 22 04:05:58", "HOSTNAME": "combo", "PID": "16663", "USERNAME": "cyrus", "UID": "0"}</t>
+          <t>{"TIMESTAMP": "Jun 22 04:05:58", "HOSTNAME": "combo", "PID": "16663", "STATE": "opened", "USERNAME": "cyrus", "UID": "0"}</t>
         </is>
       </c>
     </row>
@@ -13263,7 +13263,7 @@
       </c>
       <c r="B642" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C642" t="n">
@@ -13271,7 +13271,7 @@
       </c>
       <c r="D642" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jun 29 04:03:10", "HOSTNAME": "combo", "PID": "13665", "USERNAME": "cyrus", "UID": "0"}</t>
+          <t>{"TIMESTAMP": "Jun 29 04:03:10", "HOSTNAME": "combo", "PID": "13665", "STATE": "opened", "USERNAME": "cyrus", "UID": "0"}</t>
         </is>
       </c>
     </row>
@@ -13283,7 +13283,7 @@
       </c>
       <c r="B643" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C643" t="n">
@@ -13291,7 +13291,7 @@
       </c>
       <c r="D643" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jun 29 04:09:29", "HOSTNAME": "combo", "PID": "14891", "USERNAME": "news", "UID": "0"}</t>
+          <t>{"TIMESTAMP": "Jun 29 04:09:29", "HOSTNAME": "combo", "PID": "14891", "STATE": "opened", "USERNAME": "news", "UID": "0"}</t>
         </is>
       </c>
     </row>
@@ -13303,7 +13303,7 @@
       </c>
       <c r="B644" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C644" t="n">
@@ -13311,7 +13311,7 @@
       </c>
       <c r="D644" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul  6 04:03:08", "HOSTNAME": "combo", "PID": "8195", "USERNAME": "cyrus", "UID": "0"}</t>
+          <t>{"TIMESTAMP": "Jul  6 04:03:08", "HOSTNAME": "combo", "PID": "8195", "STATE": "opened", "USERNAME": "cyrus", "UID": "0"}</t>
         </is>
       </c>
     </row>
@@ -13323,7 +13323,7 @@
       </c>
       <c r="B645" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C645" t="n">
@@ -13331,7 +13331,7 @@
       </c>
       <c r="D645" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jun 18 04:07:05", "HOSTNAME": "combo", "PID": "31791", "USERNAME": "cyrus", "UID": "0"}</t>
+          <t>{"TIMESTAMP": "Jun 18 04:07:05", "HOSTNAME": "combo", "PID": "31791", "STATE": "opened", "USERNAME": "cyrus", "UID": "0"}</t>
         </is>
       </c>
     </row>
@@ -13343,7 +13343,7 @@
       </c>
       <c r="B646" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C646" t="n">
@@ -13351,7 +13351,7 @@
       </c>
       <c r="D646" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jun 18 04:12:42", "HOSTNAME": "combo", "PID": "32164", "USERNAME": "news", "UID": "0"}</t>
+          <t>{"TIMESTAMP": "Jun 18 04:12:42", "HOSTNAME": "combo", "PID": "32164", "STATE": "opened", "USERNAME": "news", "UID": "0"}</t>
         </is>
       </c>
     </row>
@@ -13363,7 +13363,7 @@
       </c>
       <c r="B647" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C647" t="n">
@@ -13371,7 +13371,7 @@
       </c>
       <c r="D647" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jun 19 04:08:55", "HOSTNAME": "combo", "PID": "2192", "USERNAME": "cyrus", "UID": "0"}</t>
+          <t>{"TIMESTAMP": "Jun 19 04:08:55", "HOSTNAME": "combo", "PID": "2192", "STATE": "opened", "USERNAME": "cyrus", "UID": "0"}</t>
         </is>
       </c>
     </row>
@@ -13383,7 +13383,7 @@
       </c>
       <c r="B648" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C648" t="n">
@@ -13391,7 +13391,7 @@
       </c>
       <c r="D648" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul 23 04:09:35", "HOSTNAME": "combo", "PID": "14314", "USERNAME": "cyrus", "UID": "0"}</t>
+          <t>{"TIMESTAMP": "Jul 23 04:09:35", "HOSTNAME": "combo", "PID": "14314", "STATE": "opened", "USERNAME": "cyrus", "UID": "0"}</t>
         </is>
       </c>
     </row>
@@ -13403,7 +13403,7 @@
       </c>
       <c r="B649" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C649" t="n">
@@ -13411,7 +13411,7 @@
       </c>
       <c r="D649" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul 23 04:15:13", "HOSTNAME": "combo", "PID": "14692", "USERNAME": "news", "UID": "0"}</t>
+          <t>{"TIMESTAMP": "Jul 23 04:15:13", "HOSTNAME": "combo", "PID": "14692", "STATE": "opened", "USERNAME": "news", "UID": "0"}</t>
         </is>
       </c>
     </row>
@@ -13423,7 +13423,7 @@
       </c>
       <c r="B650" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C650" t="n">
@@ -13431,7 +13431,7 @@
       </c>
       <c r="D650" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul  6 04:08:43", "HOSTNAME": "combo", "PID": "8565", "USERNAME": "news", "UID": "0"}</t>
+          <t>{"TIMESTAMP": "Jul  6 04:08:43", "HOSTNAME": "combo", "PID": "8565", "STATE": "opened", "USERNAME": "news", "UID": "0"}</t>
         </is>
       </c>
     </row>
@@ -13443,7 +13443,7 @@
       </c>
       <c r="B651" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C651" t="n">
@@ -13451,7 +13451,7 @@
       </c>
       <c r="D651" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul  1 04:05:17", "HOSTNAME": "combo", "PID": "20298", "USERNAME": "cyrus", "UID": "0"}</t>
+          <t>{"TIMESTAMP": "Jul  1 04:05:17", "HOSTNAME": "combo", "PID": "20298", "STATE": "opened", "USERNAME": "cyrus", "UID": "0"}</t>
         </is>
       </c>
     </row>
@@ -13463,7 +13463,7 @@
       </c>
       <c r="B652" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C652" t="n">
@@ -13471,7 +13471,7 @@
       </c>
       <c r="D652" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul  3 04:07:47", "HOSTNAME": "combo", "PID": "26964", "USERNAME": "cyrus", "UID": "0"}</t>
+          <t>{"TIMESTAMP": "Jul  3 04:07:47", "HOSTNAME": "combo", "PID": "26964", "STATE": "opened", "USERNAME": "cyrus", "UID": "0"}</t>
         </is>
       </c>
     </row>
@@ -13483,7 +13483,7 @@
       </c>
       <c r="B653" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C653" t="n">
@@ -13491,7 +13491,7 @@
       </c>
       <c r="D653" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul  1 04:11:35", "HOSTNAME": "combo", "PID": "21530", "USERNAME": "news", "UID": "0"}</t>
+          <t>{"TIMESTAMP": "Jul  1 04:11:35", "HOSTNAME": "combo", "PID": "21530", "STATE": "opened", "USERNAME": "news", "UID": "0"}</t>
         </is>
       </c>
     </row>
@@ -13503,7 +13503,7 @@
       </c>
       <c r="B654" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C654" t="n">
@@ -13511,7 +13511,7 @@
       </c>
       <c r="D654" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul  2 04:04:02", "HOSTNAME": "combo", "PID": "24117", "USERNAME": "cyrus", "UID": "0"}</t>
+          <t>{"TIMESTAMP": "Jul  2 04:04:02", "HOSTNAME": "combo", "PID": "24117", "STATE": "opened", "USERNAME": "cyrus", "UID": "0"}</t>
         </is>
       </c>
     </row>
@@ -13523,7 +13523,7 @@
       </c>
       <c r="B655" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C655" t="n">
@@ -13531,7 +13531,7 @@
       </c>
       <c r="D655" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul  2 04:09:53", "HOSTNAME": "combo", "PID": "24511", "USERNAME": "news", "UID": "0"}</t>
+          <t>{"TIMESTAMP": "Jul  2 04:09:53", "HOSTNAME": "combo", "PID": "24511", "STATE": "opened", "USERNAME": "news", "UID": "0"}</t>
         </is>
       </c>
     </row>
@@ -13543,7 +13543,7 @@
       </c>
       <c r="B656" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C656" t="n">
@@ -13551,7 +13551,7 @@
       </c>
       <c r="D656" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul 10 04:04:31", "HOSTNAME": "combo", "PID": "24898", "USERNAME": "cyrus", "UID": "0"}</t>
+          <t>{"TIMESTAMP": "Jul 10 04:04:31", "HOSTNAME": "combo", "PID": "24898", "STATE": "opened", "USERNAME": "cyrus", "UID": "0"}</t>
         </is>
       </c>
     </row>
@@ -13563,7 +13563,7 @@
       </c>
       <c r="B657" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C657" t="n">
@@ -13571,7 +13571,7 @@
       </c>
       <c r="D657" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul 25 04:03:58", "HOSTNAME": "combo", "PID": "24312", "USERNAME": "cyrus", "UID": "0"}</t>
+          <t>{"TIMESTAMP": "Jul 25 04:03:58", "HOSTNAME": "combo", "PID": "24312", "STATE": "opened", "USERNAME": "cyrus", "UID": "0"}</t>
         </is>
       </c>
     </row>
@@ -13583,7 +13583,7 @@
       </c>
       <c r="B658" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C658" t="n">
@@ -13591,7 +13591,7 @@
       </c>
       <c r="D658" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul 25 04:09:32", "HOSTNAME": "combo", "PID": "24683", "USERNAME": "news", "UID": "0"}</t>
+          <t>{"TIMESTAMP": "Jul 25 04:09:32", "HOSTNAME": "combo", "PID": "24683", "STATE": "opened", "USERNAME": "news", "UID": "0"}</t>
         </is>
       </c>
     </row>
@@ -13603,7 +13603,7 @@
       </c>
       <c r="B659" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C659" t="n">
@@ -13611,7 +13611,7 @@
       </c>
       <c r="D659" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul 10 04:10:47", "HOSTNAME": "combo", "PID": "26353", "USERNAME": "news", "UID": "0"}</t>
+          <t>{"TIMESTAMP": "Jul 10 04:10:47", "HOSTNAME": "combo", "PID": "26353", "STATE": "opened", "USERNAME": "news", "UID": "0"}</t>
         </is>
       </c>
     </row>
@@ -13623,7 +13623,7 @@
       </c>
       <c r="B660" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C660" t="n">
@@ -13631,7 +13631,7 @@
       </c>
       <c r="D660" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jun 21 04:06:57", "HOSTNAME": "combo", "PID": "12098", "USERNAME": "cyrus", "UID": "0"}</t>
+          <t>{"TIMESTAMP": "Jun 21 04:06:57", "HOSTNAME": "combo", "PID": "12098", "STATE": "opened", "USERNAME": "cyrus", "UID": "0"}</t>
         </is>
       </c>
     </row>
@@ -13643,7 +13643,7 @@
       </c>
       <c r="B661" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C661" t="n">
@@ -13651,7 +13651,7 @@
       </c>
       <c r="D661" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul  4 04:03:06", "HOSTNAME": "combo", "PID": "1583", "USERNAME": "cyrus", "UID": "0"}</t>
+          <t>{"TIMESTAMP": "Jul  4 04:03:06", "HOSTNAME": "combo", "PID": "1583", "STATE": "opened", "USERNAME": "cyrus", "UID": "0"}</t>
         </is>
       </c>
     </row>
@@ -13663,7 +13663,7 @@
       </c>
       <c r="B662" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C662" t="n">
@@ -13671,7 +13671,7 @@
       </c>
       <c r="D662" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul  4 04:08:48", "HOSTNAME": "combo", "PID": "1965", "USERNAME": "news", "UID": "0"}</t>
+          <t>{"TIMESTAMP": "Jul  4 04:08:48", "HOSTNAME": "combo", "PID": "1965", "STATE": "opened", "USERNAME": "news", "UID": "0"}</t>
         </is>
       </c>
     </row>
@@ -13683,7 +13683,7 @@
       </c>
       <c r="B663" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C663" t="n">
@@ -13691,7 +13691,7 @@
       </c>
       <c r="D663" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jun 21 04:13:03", "HOSTNAME": "combo", "PID": "13327", "USERNAME": "news", "UID": "0"}</t>
+          <t>{"TIMESTAMP": "Jun 21 04:13:03", "HOSTNAME": "combo", "PID": "13327", "STATE": "opened", "USERNAME": "news", "UID": "0"}</t>
         </is>
       </c>
     </row>
@@ -13703,7 +13703,7 @@
       </c>
       <c r="B664" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C664" t="n">
@@ -13711,7 +13711,7 @@
       </c>
       <c r="D664" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul 24 04:20:19", "HOSTNAME": "combo", "PID": "17283", "USERNAME": "cyrus", "UID": "0"}</t>
+          <t>{"TIMESTAMP": "Jul 24 04:20:19", "HOSTNAME": "combo", "PID": "17283", "STATE": "opened", "USERNAME": "cyrus", "UID": "0"}</t>
         </is>
       </c>
     </row>
@@ -13723,7 +13723,7 @@
       </c>
       <c r="B665" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C665" t="n">
@@ -13731,7 +13731,7 @@
       </c>
       <c r="D665" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul 26 04:05:22", "HOSTNAME": "combo", "PID": "27285", "USERNAME": "cyrus", "UID": "0"}</t>
+          <t>{"TIMESTAMP": "Jul 26 04:05:22", "HOSTNAME": "combo", "PID": "27285", "STATE": "opened", "USERNAME": "cyrus", "UID": "0"}</t>
         </is>
       </c>
     </row>
@@ -13743,7 +13743,7 @@
       </c>
       <c r="B666" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C666" t="n">
@@ -13751,7 +13751,7 @@
       </c>
       <c r="D666" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul 26 04:11:23", "HOSTNAME": "combo", "PID": "28514", "USERNAME": "news", "UID": "0"}</t>
+          <t>{"TIMESTAMP": "Jul 26 04:11:23", "HOSTNAME": "combo", "PID": "28514", "STATE": "opened", "USERNAME": "news", "UID": "0"}</t>
         </is>
       </c>
     </row>
@@ -13763,7 +13763,7 @@
       </c>
       <c r="B667" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C667" t="n">
@@ -13771,7 +13771,7 @@
       </c>
       <c r="D667" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul 24 04:33:57", "HOSTNAME": "combo", "PID": "21805", "USERNAME": "news", "UID": "0"}</t>
+          <t>{"TIMESTAMP": "Jul 24 04:33:57", "HOSTNAME": "combo", "PID": "21805", "STATE": "opened", "USERNAME": "news", "UID": "0"}</t>
         </is>
       </c>
     </row>
@@ -13783,7 +13783,7 @@
       </c>
       <c r="B668" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C668" t="n">
@@ -13791,7 +13791,7 @@
       </c>
       <c r="D668" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul  7 04:04:31", "HOSTNAME": "combo", "PID": "10961", "USERNAME": "cyrus", "UID": "0"}</t>
+          <t>{"TIMESTAMP": "Jul  7 04:04:31", "HOSTNAME": "combo", "PID": "10961", "STATE": "opened", "USERNAME": "cyrus", "UID": "0"}</t>
         </is>
       </c>
     </row>
@@ -13803,7 +13803,7 @@
       </c>
       <c r="B669" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C669" t="n">
@@ -13811,7 +13811,7 @@
       </c>
       <c r="D669" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul  7 04:10:44", "HOSTNAME": "combo", "PID": "12193", "USERNAME": "news", "UID": "0"}</t>
+          <t>{"TIMESTAMP": "Jul  7 04:10:44", "HOSTNAME": "combo", "PID": "12193", "STATE": "opened", "USERNAME": "news", "UID": "0"}</t>
         </is>
       </c>
     </row>
@@ -13823,7 +13823,7 @@
       </c>
       <c r="B670" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C670" t="n">
@@ -13831,7 +13831,7 @@
       </c>
       <c r="D670" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jun 30 04:03:41", "HOSTNAME": "combo", "PID": "17407", "USERNAME": "cyrus", "UID": "0"}</t>
+          <t>{"TIMESTAMP": "Jun 30 04:03:41", "HOSTNAME": "combo", "PID": "17407", "STATE": "opened", "USERNAME": "cyrus", "UID": "0"}</t>
         </is>
       </c>
     </row>
@@ -13843,7 +13843,7 @@
       </c>
       <c r="B671" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C671" t="n">
@@ -13851,7 +13851,7 @@
       </c>
       <c r="D671" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul  5 04:09:29", "HOSTNAME": "combo", "PID": "5699", "USERNAME": "news", "UID": "0"}</t>
+          <t>{"TIMESTAMP": "Jul  5 04:09:29", "HOSTNAME": "combo", "PID": "5699", "STATE": "opened", "USERNAME": "news", "UID": "0"}</t>
         </is>
       </c>
     </row>
@@ -13863,7 +13863,7 @@
       </c>
       <c r="B672" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C672" t="n">
@@ -13871,7 +13871,7 @@
       </c>
       <c r="D672" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul 19 04:03:43", "HOSTNAME": "combo", "PID": "29758", "USERNAME": "cyrus", "UID": "0"}</t>
+          <t>{"TIMESTAMP": "Jul 19 04:03:43", "HOSTNAME": "combo", "PID": "29758", "STATE": "opened", "USERNAME": "cyrus", "UID": "0"}</t>
         </is>
       </c>
     </row>
@@ -13883,7 +13883,7 @@
       </c>
       <c r="B673" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C673" t="n">
@@ -13891,7 +13891,7 @@
       </c>
       <c r="D673" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jun 16 04:10:22", "HOSTNAME": "combo", "PID": "25178", "USERNAME": "cyrus", "UID": "0"}</t>
+          <t>{"TIMESTAMP": "Jun 16 04:10:22", "HOSTNAME": "combo", "PID": "25178", "STATE": "opened", "USERNAME": "cyrus", "UID": "0"}</t>
         </is>
       </c>
     </row>
@@ -13903,7 +13903,7 @@
       </c>
       <c r="B674" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C674" t="n">
@@ -13911,7 +13911,7 @@
       </c>
       <c r="D674" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jun 16 04:16:17", "HOSTNAME": "combo", "PID": "25548", "USERNAME": "news", "UID": "0"}</t>
+          <t>{"TIMESTAMP": "Jun 16 04:16:17", "HOSTNAME": "combo", "PID": "25548", "STATE": "opened", "USERNAME": "news", "UID": "0"}</t>
         </is>
       </c>
     </row>
@@ -13923,7 +13923,7 @@
       </c>
       <c r="B675" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C675" t="n">
@@ -13931,7 +13931,7 @@
       </c>
       <c r="D675" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul 19 04:09:28", "HOSTNAME": "combo", "PID": "30128", "USERNAME": "news", "UID": "0"}</t>
+          <t>{"TIMESTAMP": "Jul 19 04:09:28", "HOSTNAME": "combo", "PID": "30128", "STATE": "opened", "USERNAME": "news", "UID": "0"}</t>
         </is>
       </c>
     </row>
@@ -13943,7 +13943,7 @@
       </c>
       <c r="B676" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C676" t="n">
@@ -13951,7 +13951,7 @@
       </c>
       <c r="D676" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jun 17 04:09:43", "HOSTNAME": "combo", "PID": "29190", "USERNAME": "news", "UID": "0"}</t>
+          <t>{"TIMESTAMP": "Jun 17 04:09:43", "HOSTNAME": "combo", "PID": "29190", "STATE": "opened", "USERNAME": "news", "UID": "0"}</t>
         </is>
       </c>
     </row>
@@ -13963,7 +13963,7 @@
       </c>
       <c r="B677" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C677" t="n">
@@ -13971,7 +13971,7 @@
       </c>
       <c r="D677" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jun 20 04:02:54", "HOSTNAME": "combo", "PID": "9187", "USERNAME": "cyrus", "UID": "0"}</t>
+          <t>{"TIMESTAMP": "Jun 20 04:02:54", "HOSTNAME": "combo", "PID": "9187", "STATE": "opened", "USERNAME": "cyrus", "UID": "0"}</t>
         </is>
       </c>
     </row>
@@ -13983,7 +13983,7 @@
       </c>
       <c r="B678" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C678" t="n">
@@ -13991,7 +13991,7 @@
       </c>
       <c r="D678" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jun 20 04:08:37", "HOSTNAME": "combo", "PID": "9558", "USERNAME": "news", "UID": "0"}</t>
+          <t>{"TIMESTAMP": "Jun 20 04:08:37", "HOSTNAME": "combo", "PID": "9558", "STATE": "opened", "USERNAME": "news", "UID": "0"}</t>
         </is>
       </c>
     </row>
@@ -14003,7 +14003,7 @@
       </c>
       <c r="B679" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C679" t="n">
@@ -14011,7 +14011,7 @@
       </c>
       <c r="D679" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul  8 04:04:19", "HOSTNAME": "combo", "PID": "14943", "USERNAME": "cyrus", "UID": "0"}</t>
+          <t>{"TIMESTAMP": "Jul  8 04:04:19", "HOSTNAME": "combo", "PID": "14943", "STATE": "opened", "USERNAME": "cyrus", "UID": "0"}</t>
         </is>
       </c>
     </row>
@@ -14023,7 +14023,7 @@
       </c>
       <c r="B680" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C680" t="n">
@@ -14031,7 +14031,7 @@
       </c>
       <c r="D680" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul  8 04:12:07", "HOSTNAME": "combo", "PID": "19593", "USERNAME": "news", "UID": "0"}</t>
+          <t>{"TIMESTAMP": "Jul  8 04:12:07", "HOSTNAME": "combo", "PID": "19593", "STATE": "opened", "USERNAME": "news", "UID": "0"}</t>
         </is>
       </c>
     </row>
@@ -14043,7 +14043,7 @@
       </c>
       <c r="B681" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C681" t="n">
@@ -14051,7 +14051,7 @@
       </c>
       <c r="D681" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul 20 04:05:02", "HOSTNAME": "combo", "PID": "363", "USERNAME": "cyrus", "UID": "0"}</t>
+          <t>{"TIMESTAMP": "Jul 20 04:05:02", "HOSTNAME": "combo", "PID": "363", "STATE": "opened", "USERNAME": "cyrus", "UID": "0"}</t>
         </is>
       </c>
     </row>
@@ -14063,7 +14063,7 @@
       </c>
       <c r="B682" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C682" t="n">
@@ -14071,7 +14071,7 @@
       </c>
       <c r="D682" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul  5 04:03:16", "HOSTNAME": "combo", "PID": "4474", "USERNAME": "cyrus", "UID": "0"}</t>
+          <t>{"TIMESTAMP": "Jul  5 04:03:16", "HOSTNAME": "combo", "PID": "4474", "STATE": "opened", "USERNAME": "cyrus", "UID": "0"}</t>
         </is>
       </c>
     </row>
@@ -14083,7 +14083,7 @@
       </c>
       <c r="B683" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C683" t="n">
@@ -14091,7 +14091,7 @@
       </c>
       <c r="D683" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jun 19 04:15:18", "HOSTNAME": "combo", "PID": "3676", "USERNAME": "news", "UID": "0"}</t>
+          <t>{"TIMESTAMP": "Jun 19 04:15:18", "HOSTNAME": "combo", "PID": "3676", "STATE": "opened", "USERNAME": "news", "UID": "0"}</t>
         </is>
       </c>
     </row>
@@ -14103,7 +14103,7 @@
       </c>
       <c r="B684" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C684" t="n">
@@ -14111,7 +14111,7 @@
       </c>
       <c r="D684" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul 20 04:11:27", "HOSTNAME": "combo", "PID": "1595", "USERNAME": "news", "UID": "0"}</t>
+          <t>{"TIMESTAMP": "Jul 20 04:11:27", "HOSTNAME": "combo", "PID": "1595", "STATE": "opened", "USERNAME": "news", "UID": "0"}</t>
         </is>
       </c>
     </row>
@@ -14123,7 +14123,7 @@
       </c>
       <c r="B685" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C685" t="n">
@@ -14131,7 +14131,7 @@
       </c>
       <c r="D685" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jun 30 04:09:30", "HOSTNAME": "combo", "PID": "17778", "USERNAME": "news", "UID": "0"}</t>
+          <t>{"TIMESTAMP": "Jun 30 04:09:30", "HOSTNAME": "combo", "PID": "17778", "STATE": "opened", "USERNAME": "news", "UID": "0"}</t>
         </is>
       </c>
     </row>
@@ -14143,7 +14143,7 @@
       </c>
       <c r="B686" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C686" t="n">
@@ -14151,7 +14151,7 @@
       </c>
       <c r="D686" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul 22 04:07:46", "HOSTNAME": "combo", "PID": "7106", "USERNAME": "cyrus", "UID": "0"}</t>
+          <t>{"TIMESTAMP": "Jul 22 04:07:46", "HOSTNAME": "combo", "PID": "7106", "STATE": "opened", "USERNAME": "cyrus", "UID": "0"}</t>
         </is>
       </c>
     </row>
@@ -14163,7 +14163,7 @@
       </c>
       <c r="B687" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C687" t="n">
@@ -14171,7 +14171,7 @@
       </c>
       <c r="D687" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul 22 04:15:14", "HOSTNAME": "combo", "PID": "11756", "USERNAME": "news", "UID": "0"}</t>
+          <t>{"TIMESTAMP": "Jul 22 04:15:14", "HOSTNAME": "combo", "PID": "11756", "STATE": "opened", "USERNAME": "news", "UID": "0"}</t>
         </is>
       </c>
     </row>
@@ -14183,7 +14183,7 @@
       </c>
       <c r="B688" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C688" t="n">
@@ -14191,7 +14191,7 @@
       </c>
       <c r="D688" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul 21 04:11:26", "HOSTNAME": "combo", "PID": "4170", "USERNAME": "cyrus", "UID": "0"}</t>
+          <t>{"TIMESTAMP": "Jul 21 04:11:26", "HOSTNAME": "combo", "PID": "4170", "STATE": "opened", "USERNAME": "cyrus", "UID": "0"}</t>
         </is>
       </c>
     </row>
@@ -14203,7 +14203,7 @@
       </c>
       <c r="B689" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C689" t="n">
@@ -14211,7 +14211,7 @@
       </c>
       <c r="D689" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul  9 04:04:23", "HOSTNAME": "combo", "PID": "21991", "USERNAME": "cyrus", "UID": "0"}</t>
+          <t>{"TIMESTAMP": "Jul  9 04:04:23", "HOSTNAME": "combo", "PID": "21991", "STATE": "opened", "USERNAME": "cyrus", "UID": "0"}</t>
         </is>
       </c>
     </row>
@@ -14223,7 +14223,7 @@
       </c>
       <c r="B690" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C690" t="n">
@@ -14231,7 +14231,7 @@
       </c>
       <c r="D690" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul  9 04:10:11", "HOSTNAME": "combo", "PID": "22368", "USERNAME": "news", "UID": "0"}</t>
+          <t>{"TIMESTAMP": "Jul  9 04:10:11", "HOSTNAME": "combo", "PID": "22368", "STATE": "opened", "USERNAME": "news", "UID": "0"}</t>
         </is>
       </c>
     </row>
@@ -14243,7 +14243,7 @@
       </c>
       <c r="B691" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C691" t="n">
@@ -14251,7 +14251,7 @@
       </c>
       <c r="D691" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul 21 04:16:55", "HOSTNAME": "combo", "PID": "4540", "USERNAME": "news", "UID": "0"}</t>
+          <t>{"TIMESTAMP": "Jul 21 04:16:55", "HOSTNAME": "combo", "PID": "4540", "STATE": "opened", "USERNAME": "news", "UID": "0"}</t>
         </is>
       </c>
     </row>
@@ -14263,7 +14263,7 @@
       </c>
       <c r="B692" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C692" t="n">
@@ -14271,7 +14271,7 @@
       </c>
       <c r="D692" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jun 17 04:03:33", "HOSTNAME": "combo", "PID": "27953", "USERNAME": "cyrus", "UID": "0"}</t>
+          <t>{"TIMESTAMP": "Jun 17 04:03:33", "HOSTNAME": "combo", "PID": "27953", "STATE": "opened", "USERNAME": "cyrus", "UID": "0"}</t>
         </is>
       </c>
     </row>
@@ -14283,7 +14283,7 @@
       </c>
       <c r="B693" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C693" t="n">
@@ -14291,7 +14291,7 @@
       </c>
       <c r="D693" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jun 15 04:06:19", "HOSTNAME": "combo", "PID": "21416", "USERNAME": "cyrus"}</t>
+          <t>{"TIMESTAMP": "Jun 15 04:06:19", "HOSTNAME": "combo", "PID": "21416", "STATE": "closed", "USERNAME": "cyrus"}</t>
         </is>
       </c>
     </row>
@@ -14303,7 +14303,7 @@
       </c>
       <c r="B694" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C694" t="n">
@@ -14311,7 +14311,7 @@
       </c>
       <c r="D694" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul 27 04:21:40", "HOSTNAME": "combo", "PID": "31373", "USERNAME": "news"}</t>
+          <t>{"TIMESTAMP": "Jul 27 04:21:40", "HOSTNAME": "combo", "PID": "31373", "STATE": "closed", "USERNAME": "news"}</t>
         </is>
       </c>
     </row>
@@ -14323,7 +14323,7 @@
       </c>
       <c r="B695" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C695" t="n">
@@ -14331,7 +14331,7 @@
       </c>
       <c r="D695" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jun 15 04:12:43", "HOSTNAME": "combo", "PID": "22644", "USERNAME": "news"}</t>
+          <t>{"TIMESTAMP": "Jun 15 04:12:43", "HOSTNAME": "combo", "PID": "22644", "STATE": "closed", "USERNAME": "news"}</t>
         </is>
       </c>
     </row>
@@ -14343,7 +14343,7 @@
       </c>
       <c r="B696" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C696" t="n">
@@ -14351,7 +14351,7 @@
       </c>
       <c r="D696" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul  4 04:03:07", "HOSTNAME": "combo", "PID": "1583", "USERNAME": "cyrus"}</t>
+          <t>{"TIMESTAMP": "Jul  4 04:03:07", "HOSTNAME": "combo", "PID": "1583", "STATE": "closed", "USERNAME": "cyrus"}</t>
         </is>
       </c>
     </row>
@@ -14363,7 +14363,7 @@
       </c>
       <c r="B697" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C697" t="n">
@@ -14371,7 +14371,7 @@
       </c>
       <c r="D697" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul  4 04:08:49", "HOSTNAME": "combo", "PID": "1965", "USERNAME": "news"}</t>
+          <t>{"TIMESTAMP": "Jul  4 04:08:49", "HOSTNAME": "combo", "PID": "1965", "STATE": "closed", "USERNAME": "news"}</t>
         </is>
       </c>
     </row>
@@ -14383,7 +14383,7 @@
       </c>
       <c r="B698" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C698" t="n">
@@ -14391,7 +14391,7 @@
       </c>
       <c r="D698" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul  5 04:03:17", "HOSTNAME": "combo", "PID": "4474", "USERNAME": "cyrus"}</t>
+          <t>{"TIMESTAMP": "Jul  5 04:03:17", "HOSTNAME": "combo", "PID": "4474", "STATE": "closed", "USERNAME": "cyrus"}</t>
         </is>
       </c>
     </row>
@@ -14403,7 +14403,7 @@
       </c>
       <c r="B699" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C699" t="n">
@@ -14411,7 +14411,7 @@
       </c>
       <c r="D699" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul 14 04:14:39", "HOSTNAME": "combo", "PID": "10583", "USERNAME": "news"}</t>
+          <t>{"TIMESTAMP": "Jul 14 04:14:39", "HOSTNAME": "combo", "PID": "10583", "STATE": "closed", "USERNAME": "news"}</t>
         </is>
       </c>
     </row>
@@ -14423,7 +14423,7 @@
       </c>
       <c r="B700" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C700" t="n">
@@ -14431,7 +14431,7 @@
       </c>
       <c r="D700" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul 14 04:08:25", "HOSTNAME": "combo", "PID": "9355", "USERNAME": "cyrus"}</t>
+          <t>{"TIMESTAMP": "Jul 14 04:08:25", "HOSTNAME": "combo", "PID": "9355", "STATE": "closed", "USERNAME": "cyrus"}</t>
         </is>
       </c>
     </row>
@@ -14443,7 +14443,7 @@
       </c>
       <c r="B701" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C701" t="n">
@@ -14451,7 +14451,7 @@
       </c>
       <c r="D701" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul 13 04:04:45", "HOSTNAME": "combo", "PID": "6486", "USERNAME": "cyrus"}</t>
+          <t>{"TIMESTAMP": "Jul 13 04:04:45", "HOSTNAME": "combo", "PID": "6486", "STATE": "closed", "USERNAME": "cyrus"}</t>
         </is>
       </c>
     </row>
@@ -14463,7 +14463,7 @@
       </c>
       <c r="B702" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C702" t="n">
@@ -14471,7 +14471,7 @@
       </c>
       <c r="D702" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul 13 04:10:41", "HOSTNAME": "combo", "PID": "6863", "USERNAME": "news"}</t>
+          <t>{"TIMESTAMP": "Jul 13 04:10:41", "HOSTNAME": "combo", "PID": "6863", "STATE": "closed", "USERNAME": "news"}</t>
         </is>
       </c>
     </row>
@@ -14483,7 +14483,7 @@
       </c>
       <c r="B703" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C703" t="n">
@@ -14491,7 +14491,7 @@
       </c>
       <c r="D703" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul 12 04:09:50", "HOSTNAME": "combo", "PID": "3833", "USERNAME": "news"}</t>
+          <t>{"TIMESTAMP": "Jul 12 04:09:50", "HOSTNAME": "combo", "PID": "3833", "STATE": "closed", "USERNAME": "news"}</t>
         </is>
       </c>
     </row>
@@ -14503,7 +14503,7 @@
       </c>
       <c r="B704" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C704" t="n">
@@ -14511,7 +14511,7 @@
       </c>
       <c r="D704" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul 12 04:03:41", "HOSTNAME": "combo", "PID": "2605", "USERNAME": "cyrus"}</t>
+          <t>{"TIMESTAMP": "Jul 12 04:03:41", "HOSTNAME": "combo", "PID": "2605", "STATE": "closed", "USERNAME": "cyrus"}</t>
         </is>
       </c>
     </row>
@@ -14523,7 +14523,7 @@
       </c>
       <c r="B705" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C705" t="n">
@@ -14531,7 +14531,7 @@
       </c>
       <c r="D705" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul 11 04:03:04", "HOSTNAME": "combo", "PID": "32237", "USERNAME": "cyrus"}</t>
+          <t>{"TIMESTAMP": "Jul 11 04:03:04", "HOSTNAME": "combo", "PID": "32237", "STATE": "closed", "USERNAME": "cyrus"}</t>
         </is>
       </c>
     </row>
@@ -14543,7 +14543,7 @@
       </c>
       <c r="B706" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C706" t="n">
@@ -14551,7 +14551,7 @@
       </c>
       <c r="D706" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul 11 04:08:38", "HOSTNAME": "combo", "PID": "32608", "USERNAME": "news"}</t>
+          <t>{"TIMESTAMP": "Jul 11 04:08:38", "HOSTNAME": "combo", "PID": "32608", "STATE": "closed", "USERNAME": "news"}</t>
         </is>
       </c>
     </row>
@@ -14563,7 +14563,7 @@
       </c>
       <c r="B707" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C707" t="n">
@@ -14571,7 +14571,7 @@
       </c>
       <c r="D707" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jun 28 04:03:16", "HOSTNAME": "combo", "PID": "10735", "USERNAME": "cyrus"}</t>
+          <t>{"TIMESTAMP": "Jun 28 04:03:16", "HOSTNAME": "combo", "PID": "10735", "STATE": "closed", "USERNAME": "cyrus"}</t>
         </is>
       </c>
     </row>
@@ -14583,7 +14583,7 @@
       </c>
       <c r="B708" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C708" t="n">
@@ -14591,7 +14591,7 @@
       </c>
       <c r="D708" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jun 28 04:09:01", "HOSTNAME": "combo", "PID": "11106", "USERNAME": "news"}</t>
+          <t>{"TIMESTAMP": "Jun 28 04:09:01", "HOSTNAME": "combo", "PID": "11106", "STATE": "closed", "USERNAME": "news"}</t>
         </is>
       </c>
     </row>
@@ -14603,7 +14603,7 @@
       </c>
       <c r="B709" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C709" t="n">
@@ -14611,7 +14611,7 @@
       </c>
       <c r="D709" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jun 27 04:02:48", "HOSTNAME": "combo", "PID": "7031", "USERNAME": "cyrus"}</t>
+          <t>{"TIMESTAMP": "Jun 27 04:02:48", "HOSTNAME": "combo", "PID": "7031", "STATE": "closed", "USERNAME": "cyrus"}</t>
         </is>
       </c>
     </row>
@@ -14623,7 +14623,7 @@
       </c>
       <c r="B710" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C710" t="n">
@@ -14631,7 +14631,7 @@
       </c>
       <c r="D710" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jun 27 04:08:57", "HOSTNAME": "combo", "PID": "8269", "USERNAME": "news"}</t>
+          <t>{"TIMESTAMP": "Jun 27 04:08:57", "HOSTNAME": "combo", "PID": "8269", "STATE": "closed", "USERNAME": "news"}</t>
         </is>
       </c>
     </row>
@@ -14643,7 +14643,7 @@
       </c>
       <c r="B711" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C711" t="n">
@@ -14651,7 +14651,7 @@
       </c>
       <c r="D711" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jun 26 04:04:17", "HOSTNAME": "combo", "PID": "945", "USERNAME": "cyrus"}</t>
+          <t>{"TIMESTAMP": "Jun 26 04:04:17", "HOSTNAME": "combo", "PID": "945", "STATE": "closed", "USERNAME": "cyrus"}</t>
         </is>
       </c>
     </row>
@@ -14663,7 +14663,7 @@
       </c>
       <c r="B712" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C712" t="n">
@@ -14671,7 +14671,7 @@
       </c>
       <c r="D712" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jun 26 04:10:04", "HOSTNAME": "combo", "PID": "1546", "USERNAME": "news"}</t>
+          <t>{"TIMESTAMP": "Jun 26 04:10:04", "HOSTNAME": "combo", "PID": "1546", "STATE": "closed", "USERNAME": "news"}</t>
         </is>
       </c>
     </row>
@@ -14683,7 +14683,7 @@
       </c>
       <c r="B713" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C713" t="n">
@@ -14691,7 +14691,7 @@
       </c>
       <c r="D713" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jun 29 04:03:11", "HOSTNAME": "combo", "PID": "13665", "USERNAME": "cyrus"}</t>
+          <t>{"TIMESTAMP": "Jun 29 04:03:11", "HOSTNAME": "combo", "PID": "13665", "STATE": "closed", "USERNAME": "cyrus"}</t>
         </is>
       </c>
     </row>
@@ -14703,7 +14703,7 @@
       </c>
       <c r="B714" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C714" t="n">
@@ -14711,7 +14711,7 @@
       </c>
       <c r="D714" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jun 29 04:09:30", "HOSTNAME": "combo", "PID": "14891", "USERNAME": "news"}</t>
+          <t>{"TIMESTAMP": "Jun 29 04:09:30", "HOSTNAME": "combo", "PID": "14891", "STATE": "closed", "USERNAME": "news"}</t>
         </is>
       </c>
     </row>
@@ -14723,7 +14723,7 @@
       </c>
       <c r="B715" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C715" t="n">
@@ -14731,7 +14731,7 @@
       </c>
       <c r="D715" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jun 30 04:03:42", "HOSTNAME": "combo", "PID": "17407", "USERNAME": "cyrus"}</t>
+          <t>{"TIMESTAMP": "Jun 30 04:03:42", "HOSTNAME": "combo", "PID": "17407", "STATE": "closed", "USERNAME": "cyrus"}</t>
         </is>
       </c>
     </row>
@@ -14743,7 +14743,7 @@
       </c>
       <c r="B716" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C716" t="n">
@@ -14751,7 +14751,7 @@
       </c>
       <c r="D716" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jun 30 04:09:31", "HOSTNAME": "combo", "PID": "17778", "USERNAME": "news"}</t>
+          <t>{"TIMESTAMP": "Jun 30 04:09:31", "HOSTNAME": "combo", "PID": "17778", "STATE": "closed", "USERNAME": "news"}</t>
         </is>
       </c>
     </row>
@@ -14763,7 +14763,7 @@
       </c>
       <c r="B717" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C717" t="n">
@@ -14771,7 +14771,7 @@
       </c>
       <c r="D717" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul  3 04:14:01", "HOSTNAME": "combo", "PID": "28416", "USERNAME": "news"}</t>
+          <t>{"TIMESTAMP": "Jul  3 04:14:01", "HOSTNAME": "combo", "PID": "28416", "STATE": "closed", "USERNAME": "news"}</t>
         </is>
       </c>
     </row>
@@ -14783,7 +14783,7 @@
       </c>
       <c r="B718" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C718" t="n">
@@ -14791,7 +14791,7 @@
       </c>
       <c r="D718" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul  3 04:07:48", "HOSTNAME": "combo", "PID": "26964", "USERNAME": "cyrus"}</t>
+          <t>{"TIMESTAMP": "Jul  3 04:07:48", "HOSTNAME": "combo", "PID": "26964", "STATE": "closed", "USERNAME": "cyrus"}</t>
         </is>
       </c>
     </row>
@@ -14803,7 +14803,7 @@
       </c>
       <c r="B719" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C719" t="n">
@@ -14811,7 +14811,7 @@
       </c>
       <c r="D719" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul 17 04:13:58", "HOSTNAME": "combo", "PID": "20282", "USERNAME": "news"}</t>
+          <t>{"TIMESTAMP": "Jul 17 04:13:58", "HOSTNAME": "combo", "PID": "20282", "STATE": "closed", "USERNAME": "news"}</t>
         </is>
       </c>
     </row>
@@ -14823,7 +14823,7 @@
       </c>
       <c r="B720" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C720" t="n">
@@ -14831,7 +14831,7 @@
       </c>
       <c r="D720" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul 16 04:14:00", "HOSTNAME": "combo", "PID": "17286", "USERNAME": "news"}</t>
+          <t>{"TIMESTAMP": "Jul 16 04:14:00", "HOSTNAME": "combo", "PID": "17286", "STATE": "closed", "USERNAME": "news"}</t>
         </is>
       </c>
     </row>
@@ -14843,7 +14843,7 @@
       </c>
       <c r="B721" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C721" t="n">
@@ -14851,7 +14851,7 @@
       </c>
       <c r="D721" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul 16 04:07:33", "HOSTNAME": "combo", "PID": "16058", "USERNAME": "cyrus"}</t>
+          <t>{"TIMESTAMP": "Jul 16 04:07:33", "HOSTNAME": "combo", "PID": "16058", "STATE": "closed", "USERNAME": "cyrus"}</t>
         </is>
       </c>
     </row>
@@ -14863,7 +14863,7 @@
       </c>
       <c r="B722" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C722" t="n">
@@ -14871,7 +14871,7 @@
       </c>
       <c r="D722" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jun 25 04:10:35", "HOSTNAME": "combo", "PID": "30934", "USERNAME": "news"}</t>
+          <t>{"TIMESTAMP": "Jun 25 04:10:35", "HOSTNAME": "combo", "PID": "30934", "STATE": "closed", "USERNAME": "news"}</t>
         </is>
       </c>
     </row>
@@ -14883,7 +14883,7 @@
       </c>
       <c r="B723" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C723" t="n">
@@ -14891,7 +14891,7 @@
       </c>
       <c r="D723" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jun 25 04:04:25", "HOSTNAME": "combo", "PID": "29690", "USERNAME": "cyrus"}</t>
+          <t>{"TIMESTAMP": "Jun 25 04:04:25", "HOSTNAME": "combo", "PID": "29690", "STATE": "closed", "USERNAME": "cyrus"}</t>
         </is>
       </c>
     </row>
@@ -14903,7 +14903,7 @@
       </c>
       <c r="B724" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C724" t="n">
@@ -14911,7 +14911,7 @@
       </c>
       <c r="D724" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jun 24 04:05:35", "HOSTNAME": "combo", "PID": "26938", "USERNAME": "cyrus"}</t>
+          <t>{"TIMESTAMP": "Jun 24 04:05:35", "HOSTNAME": "combo", "PID": "26938", "STATE": "closed", "USERNAME": "cyrus"}</t>
         </is>
       </c>
     </row>
@@ -14923,7 +14923,7 @@
       </c>
       <c r="B725" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C725" t="n">
@@ -14931,7 +14931,7 @@
       </c>
       <c r="D725" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jun 24 04:11:12", "HOSTNAME": "combo", "PID": "27311", "USERNAME": "news"}</t>
+          <t>{"TIMESTAMP": "Jun 24 04:11:12", "HOSTNAME": "combo", "PID": "27311", "STATE": "closed", "USERNAME": "news"}</t>
         </is>
       </c>
     </row>
@@ -14943,7 +14943,7 @@
       </c>
       <c r="B726" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C726" t="n">
@@ -14951,7 +14951,7 @@
       </c>
       <c r="D726" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul 15 04:05:02", "HOSTNAME": "combo", "PID": "13238", "USERNAME": "cyrus"}</t>
+          <t>{"TIMESTAMP": "Jul 15 04:05:02", "HOSTNAME": "combo", "PID": "13238", "STATE": "closed", "USERNAME": "cyrus"}</t>
         </is>
       </c>
     </row>
@@ -14963,7 +14963,7 @@
       </c>
       <c r="B727" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C727" t="n">
@@ -14971,7 +14971,7 @@
       </c>
       <c r="D727" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul 15 04:10:46", "HOSTNAME": "combo", "PID": "13611", "USERNAME": "news"}</t>
+          <t>{"TIMESTAMP": "Jul 15 04:10:46", "HOSTNAME": "combo", "PID": "13611", "STATE": "closed", "USERNAME": "news"}</t>
         </is>
       </c>
     </row>
@@ -14983,7 +14983,7 @@
       </c>
       <c r="B728" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C728" t="n">
@@ -14991,7 +14991,7 @@
       </c>
       <c r="D728" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul  5 04:09:30", "HOSTNAME": "combo", "PID": "5699", "USERNAME": "news"}</t>
+          <t>{"TIMESTAMP": "Jul  5 04:09:30", "HOSTNAME": "combo", "PID": "5699", "STATE": "closed", "USERNAME": "news"}</t>
         </is>
       </c>
     </row>
@@ -15003,7 +15003,7 @@
       </c>
       <c r="B729" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C729" t="n">
@@ -15011,7 +15011,7 @@
       </c>
       <c r="D729" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul 26 04:11:23", "HOSTNAME": "combo", "PID": "28514", "USERNAME": "news"}</t>
+          <t>{"TIMESTAMP": "Jul 26 04:11:23", "HOSTNAME": "combo", "PID": "28514", "STATE": "closed", "USERNAME": "news"}</t>
         </is>
       </c>
     </row>
@@ -15023,7 +15023,7 @@
       </c>
       <c r="B730" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C730" t="n">
@@ -15031,7 +15031,7 @@
       </c>
       <c r="D730" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul 25 04:03:59", "HOSTNAME": "combo", "PID": "24312", "USERNAME": "cyrus"}</t>
+          <t>{"TIMESTAMP": "Jul 25 04:03:59", "HOSTNAME": "combo", "PID": "24312", "STATE": "closed", "USERNAME": "cyrus"}</t>
         </is>
       </c>
     </row>
@@ -15043,7 +15043,7 @@
       </c>
       <c r="B731" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C731" t="n">
@@ -15051,7 +15051,7 @@
       </c>
       <c r="D731" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul 25 04:09:33", "HOSTNAME": "combo", "PID": "24683", "USERNAME": "news"}</t>
+          <t>{"TIMESTAMP": "Jul 25 04:09:33", "HOSTNAME": "combo", "PID": "24683", "STATE": "closed", "USERNAME": "news"}</t>
         </is>
       </c>
     </row>
@@ -15063,7 +15063,7 @@
       </c>
       <c r="B732" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C732" t="n">
@@ -15071,7 +15071,7 @@
       </c>
       <c r="D732" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul 24 04:33:58", "HOSTNAME": "combo", "PID": "21805", "USERNAME": "news"}</t>
+          <t>{"TIMESTAMP": "Jul 24 04:33:58", "HOSTNAME": "combo", "PID": "21805", "STATE": "closed", "USERNAME": "news"}</t>
         </is>
       </c>
     </row>
@@ -15083,7 +15083,7 @@
       </c>
       <c r="B733" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C733" t="n">
@@ -15091,7 +15091,7 @@
       </c>
       <c r="D733" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul 24 04:20:19", "HOSTNAME": "combo", "PID": "17283", "USERNAME": "cyrus"}</t>
+          <t>{"TIMESTAMP": "Jul 24 04:20:19", "HOSTNAME": "combo", "PID": "17283", "STATE": "closed", "USERNAME": "cyrus"}</t>
         </is>
       </c>
     </row>
@@ -15103,7 +15103,7 @@
       </c>
       <c r="B734" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C734" t="n">
@@ -15111,7 +15111,7 @@
       </c>
       <c r="D734" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul 23 04:15:13", "HOSTNAME": "combo", "PID": "14692", "USERNAME": "news"}</t>
+          <t>{"TIMESTAMP": "Jul 23 04:15:13", "HOSTNAME": "combo", "PID": "14692", "STATE": "closed", "USERNAME": "news"}</t>
         </is>
       </c>
     </row>
@@ -15123,7 +15123,7 @@
       </c>
       <c r="B735" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C735" t="n">
@@ -15131,7 +15131,7 @@
       </c>
       <c r="D735" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul 23 04:09:36", "HOSTNAME": "combo", "PID": "14314", "USERNAME": "cyrus"}</t>
+          <t>{"TIMESTAMP": "Jul 23 04:09:36", "HOSTNAME": "combo", "PID": "14314", "STATE": "closed", "USERNAME": "cyrus"}</t>
         </is>
       </c>
     </row>
@@ -15143,7 +15143,7 @@
       </c>
       <c r="B736" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C736" t="n">
@@ -15151,7 +15151,7 @@
       </c>
       <c r="D736" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul 10 04:04:32", "HOSTNAME": "combo", "PID": "24898", "USERNAME": "cyrus"}</t>
+          <t>{"TIMESTAMP": "Jul 10 04:04:32", "HOSTNAME": "combo", "PID": "24898", "STATE": "closed", "USERNAME": "cyrus"}</t>
         </is>
       </c>
     </row>
@@ -15163,7 +15163,7 @@
       </c>
       <c r="B737" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C737" t="n">
@@ -15171,7 +15171,7 @@
       </c>
       <c r="D737" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul 17 04:08:09", "HOSTNAME": "combo", "PID": "19686", "USERNAME": "cyrus"}</t>
+          <t>{"TIMESTAMP": "Jul 17 04:08:09", "HOSTNAME": "combo", "PID": "19686", "STATE": "closed", "USERNAME": "cyrus"}</t>
         </is>
       </c>
     </row>
@@ -15183,7 +15183,7 @@
       </c>
       <c r="B738" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C738" t="n">
@@ -15191,7 +15191,7 @@
       </c>
       <c r="D738" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul 10 04:10:47", "HOSTNAME": "combo", "PID": "26353", "USERNAME": "news"}</t>
+          <t>{"TIMESTAMP": "Jul 10 04:10:47", "HOSTNAME": "combo", "PID": "26353", "STATE": "closed", "USERNAME": "news"}</t>
         </is>
       </c>
     </row>
@@ -15203,7 +15203,7 @@
       </c>
       <c r="B739" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C739" t="n">
@@ -15211,7 +15211,7 @@
       </c>
       <c r="D739" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul  1 04:05:18", "HOSTNAME": "combo", "PID": "20298", "USERNAME": "cyrus"}</t>
+          <t>{"TIMESTAMP": "Jul  1 04:05:18", "HOSTNAME": "combo", "PID": "20298", "STATE": "closed", "USERNAME": "cyrus"}</t>
         </is>
       </c>
     </row>
@@ -15223,7 +15223,7 @@
       </c>
       <c r="B740" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C740" t="n">
@@ -15231,7 +15231,7 @@
       </c>
       <c r="D740" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul  1 04:11:36", "HOSTNAME": "combo", "PID": "21530", "USERNAME": "news"}</t>
+          <t>{"TIMESTAMP": "Jul  1 04:11:36", "HOSTNAME": "combo", "PID": "21530", "STATE": "closed", "USERNAME": "news"}</t>
         </is>
       </c>
     </row>
@@ -15243,7 +15243,7 @@
       </c>
       <c r="B741" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C741" t="n">
@@ -15251,7 +15251,7 @@
       </c>
       <c r="D741" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jun 23 04:05:29", "HOSTNAME": "combo", "PID": "19534", "USERNAME": "cyrus"}</t>
+          <t>{"TIMESTAMP": "Jun 23 04:05:29", "HOSTNAME": "combo", "PID": "19534", "STATE": "closed", "USERNAME": "cyrus"}</t>
         </is>
       </c>
     </row>
@@ -15263,7 +15263,7 @@
       </c>
       <c r="B742" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C742" t="n">
@@ -15271,7 +15271,7 @@
       </c>
       <c r="D742" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jun 23 04:13:09", "HOSTNAME": "combo", "PID": "24180", "USERNAME": "news"}</t>
+          <t>{"TIMESTAMP": "Jun 23 04:13:09", "HOSTNAME": "combo", "PID": "24180", "STATE": "closed", "USERNAME": "news"}</t>
         </is>
       </c>
     </row>
@@ -15283,7 +15283,7 @@
       </c>
       <c r="B743" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C743" t="n">
@@ -15291,7 +15291,7 @@
       </c>
       <c r="D743" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul  9 04:04:24", "HOSTNAME": "combo", "PID": "21991", "USERNAME": "cyrus"}</t>
+          <t>{"TIMESTAMP": "Jul  9 04:04:24", "HOSTNAME": "combo", "PID": "21991", "STATE": "closed", "USERNAME": "cyrus"}</t>
         </is>
       </c>
     </row>
@@ -15303,7 +15303,7 @@
       </c>
       <c r="B744" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C744" t="n">
@@ -15311,7 +15311,7 @@
       </c>
       <c r="D744" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul  9 04:10:12", "HOSTNAME": "combo", "PID": "22368", "USERNAME": "news"}</t>
+          <t>{"TIMESTAMP": "Jul  9 04:10:12", "HOSTNAME": "combo", "PID": "22368", "STATE": "closed", "USERNAME": "news"}</t>
         </is>
       </c>
     </row>
@@ -15323,7 +15323,7 @@
       </c>
       <c r="B745" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C745" t="n">
@@ -15331,7 +15331,7 @@
       </c>
       <c r="D745" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul  8 04:04:19", "HOSTNAME": "combo", "PID": "14943", "USERNAME": "cyrus"}</t>
+          <t>{"TIMESTAMP": "Jul  8 04:04:19", "HOSTNAME": "combo", "PID": "14943", "STATE": "closed", "USERNAME": "cyrus"}</t>
         </is>
       </c>
     </row>
@@ -15343,7 +15343,7 @@
       </c>
       <c r="B746" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C746" t="n">
@@ -15351,7 +15351,7 @@
       </c>
       <c r="D746" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul  8 04:12:08", "HOSTNAME": "combo", "PID": "19593", "USERNAME": "news"}</t>
+          <t>{"TIMESTAMP": "Jul  8 04:12:08", "HOSTNAME": "combo", "PID": "19593", "STATE": "closed", "USERNAME": "news"}</t>
         </is>
       </c>
     </row>
@@ -15363,7 +15363,7 @@
       </c>
       <c r="B747" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C747" t="n">
@@ -15371,7 +15371,7 @@
       </c>
       <c r="D747" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jun 20 04:08:38", "HOSTNAME": "combo", "PID": "9558", "USERNAME": "news"}</t>
+          <t>{"TIMESTAMP": "Jun 20 04:08:38", "HOSTNAME": "combo", "PID": "9558", "STATE": "closed", "USERNAME": "news"}</t>
         </is>
       </c>
     </row>
@@ -15383,7 +15383,7 @@
       </c>
       <c r="B748" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C748" t="n">
@@ -15391,7 +15391,7 @@
       </c>
       <c r="D748" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul 20 04:11:28", "HOSTNAME": "combo", "PID": "1595", "USERNAME": "news"}</t>
+          <t>{"TIMESTAMP": "Jul 20 04:11:28", "HOSTNAME": "combo", "PID": "1595", "STATE": "closed", "USERNAME": "news"}</t>
         </is>
       </c>
     </row>
@@ -15403,7 +15403,7 @@
       </c>
       <c r="B749" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C749" t="n">
@@ -15411,7 +15411,7 @@
       </c>
       <c r="D749" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul 20 04:05:03", "HOSTNAME": "combo", "PID": "363", "USERNAME": "cyrus"}</t>
+          <t>{"TIMESTAMP": "Jul 20 04:05:03", "HOSTNAME": "combo", "PID": "363", "STATE": "closed", "USERNAME": "cyrus"}</t>
         </is>
       </c>
     </row>
@@ -15423,7 +15423,7 @@
       </c>
       <c r="B750" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C750" t="n">
@@ -15431,7 +15431,7 @@
       </c>
       <c r="D750" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul 19 04:03:44", "HOSTNAME": "combo", "PID": "29758", "USERNAME": "cyrus"}</t>
+          <t>{"TIMESTAMP": "Jul 19 04:03:44", "HOSTNAME": "combo", "PID": "29758", "STATE": "closed", "USERNAME": "cyrus"}</t>
         </is>
       </c>
     </row>
@@ -15443,7 +15443,7 @@
       </c>
       <c r="B751" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C751" t="n">
@@ -15451,7 +15451,7 @@
       </c>
       <c r="D751" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul 19 04:09:29", "HOSTNAME": "combo", "PID": "30128", "USERNAME": "news"}</t>
+          <t>{"TIMESTAMP": "Jul 19 04:09:29", "HOSTNAME": "combo", "PID": "30128", "STATE": "closed", "USERNAME": "news"}</t>
         </is>
       </c>
     </row>
@@ -15463,7 +15463,7 @@
       </c>
       <c r="B752" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C752" t="n">
@@ -15471,7 +15471,7 @@
       </c>
       <c r="D752" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul  6 04:08:44", "HOSTNAME": "combo", "PID": "8565", "USERNAME": "news"}</t>
+          <t>{"TIMESTAMP": "Jul  6 04:08:44", "HOSTNAME": "combo", "PID": "8565", "STATE": "closed", "USERNAME": "news"}</t>
         </is>
       </c>
     </row>
@@ -15483,7 +15483,7 @@
       </c>
       <c r="B753" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C753" t="n">
@@ -15491,7 +15491,7 @@
       </c>
       <c r="D753" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul 18 04:03:24", "HOSTNAME": "combo", "PID": "26046", "USERNAME": "cyrus"}</t>
+          <t>{"TIMESTAMP": "Jul 18 04:03:24", "HOSTNAME": "combo", "PID": "26046", "STATE": "closed", "USERNAME": "cyrus"}</t>
         </is>
       </c>
     </row>
@@ -15503,7 +15503,7 @@
       </c>
       <c r="B754" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C754" t="n">
@@ -15511,7 +15511,7 @@
       </c>
       <c r="D754" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul 18 04:09:30", "HOSTNAME": "combo", "PID": "27272", "USERNAME": "news"}</t>
+          <t>{"TIMESTAMP": "Jul 18 04:09:30", "HOSTNAME": "combo", "PID": "27272", "STATE": "closed", "USERNAME": "news"}</t>
         </is>
       </c>
     </row>
@@ -15523,7 +15523,7 @@
       </c>
       <c r="B755" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C755" t="n">
@@ -15531,7 +15531,7 @@
       </c>
       <c r="D755" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul 22 04:07:47", "HOSTNAME": "combo", "PID": "7106", "USERNAME": "cyrus"}</t>
+          <t>{"TIMESTAMP": "Jul 22 04:07:47", "HOSTNAME": "combo", "PID": "7106", "STATE": "closed", "USERNAME": "cyrus"}</t>
         </is>
       </c>
     </row>
@@ -15543,7 +15543,7 @@
       </c>
       <c r="B756" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C756" t="n">
@@ -15551,7 +15551,7 @@
       </c>
       <c r="D756" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul 22 04:15:14", "HOSTNAME": "combo", "PID": "11756", "USERNAME": "news"}</t>
+          <t>{"TIMESTAMP": "Jul 22 04:15:14", "HOSTNAME": "combo", "PID": "11756", "STATE": "closed", "USERNAME": "news"}</t>
         </is>
       </c>
     </row>
@@ -15563,7 +15563,7 @@
       </c>
       <c r="B757" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C757" t="n">
@@ -15571,7 +15571,7 @@
       </c>
       <c r="D757" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jun 18 04:12:43", "HOSTNAME": "combo", "PID": "32164", "USERNAME": "news"}</t>
+          <t>{"TIMESTAMP": "Jun 18 04:12:43", "HOSTNAME": "combo", "PID": "32164", "STATE": "closed", "USERNAME": "news"}</t>
         </is>
       </c>
     </row>
@@ -15583,7 +15583,7 @@
       </c>
       <c r="B758" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C758" t="n">
@@ -15591,7 +15591,7 @@
       </c>
       <c r="D758" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jun 19 04:08:55", "HOSTNAME": "combo", "PID": "2192", "USERNAME": "cyrus"}</t>
+          <t>{"TIMESTAMP": "Jun 19 04:08:55", "HOSTNAME": "combo", "PID": "2192", "STATE": "closed", "USERNAME": "cyrus"}</t>
         </is>
       </c>
     </row>
@@ -15603,7 +15603,7 @@
       </c>
       <c r="B759" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C759" t="n">
@@ -15611,7 +15611,7 @@
       </c>
       <c r="D759" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jun 19 04:15:18", "HOSTNAME": "combo", "PID": "3676", "USERNAME": "news"}</t>
+          <t>{"TIMESTAMP": "Jun 19 04:15:18", "HOSTNAME": "combo", "PID": "3676", "STATE": "closed", "USERNAME": "news"}</t>
         </is>
       </c>
     </row>
@@ -15623,7 +15623,7 @@
       </c>
       <c r="B760" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C760" t="n">
@@ -15631,7 +15631,7 @@
       </c>
       <c r="D760" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jun 18 04:07:06", "HOSTNAME": "combo", "PID": "31791", "USERNAME": "cyrus"}</t>
+          <t>{"TIMESTAMP": "Jun 18 04:07:06", "HOSTNAME": "combo", "PID": "31791", "STATE": "closed", "USERNAME": "cyrus"}</t>
         </is>
       </c>
     </row>
@@ -15643,7 +15643,7 @@
       </c>
       <c r="B761" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C761" t="n">
@@ -15651,7 +15651,7 @@
       </c>
       <c r="D761" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul  6 04:03:09", "HOSTNAME": "combo", "PID": "8195", "USERNAME": "cyrus"}</t>
+          <t>{"TIMESTAMP": "Jul  6 04:03:09", "HOSTNAME": "combo", "PID": "8195", "STATE": "closed", "USERNAME": "cyrus"}</t>
         </is>
       </c>
     </row>
@@ -15663,7 +15663,7 @@
       </c>
       <c r="B762" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C762" t="n">
@@ -15671,7 +15671,7 @@
       </c>
       <c r="D762" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul  7 04:04:32", "HOSTNAME": "combo", "PID": "10961", "USERNAME": "cyrus"}</t>
+          <t>{"TIMESTAMP": "Jul  7 04:04:32", "HOSTNAME": "combo", "PID": "10961", "STATE": "closed", "USERNAME": "cyrus"}</t>
         </is>
       </c>
     </row>
@@ -15683,7 +15683,7 @@
       </c>
       <c r="B763" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C763" t="n">
@@ -15691,7 +15691,7 @@
       </c>
       <c r="D763" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul  7 04:10:45", "HOSTNAME": "combo", "PID": "12193", "USERNAME": "news"}</t>
+          <t>{"TIMESTAMP": "Jul  7 04:10:45", "HOSTNAME": "combo", "PID": "12193", "STATE": "closed", "USERNAME": "news"}</t>
         </is>
       </c>
     </row>
@@ -15703,7 +15703,7 @@
       </c>
       <c r="B764" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C764" t="n">
@@ -15711,7 +15711,7 @@
       </c>
       <c r="D764" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul 21 04:11:27", "HOSTNAME": "combo", "PID": "4170", "USERNAME": "cyrus"}</t>
+          <t>{"TIMESTAMP": "Jul 21 04:11:27", "HOSTNAME": "combo", "PID": "4170", "STATE": "closed", "USERNAME": "cyrus"}</t>
         </is>
       </c>
     </row>
@@ -15723,7 +15723,7 @@
       </c>
       <c r="B765" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C765" t="n">
@@ -15731,7 +15731,7 @@
       </c>
       <c r="D765" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul 21 04:16:55", "HOSTNAME": "combo", "PID": "4540", "USERNAME": "news"}</t>
+          <t>{"TIMESTAMP": "Jul 21 04:16:55", "HOSTNAME": "combo", "PID": "4540", "STATE": "closed", "USERNAME": "news"}</t>
         </is>
       </c>
     </row>
@@ -15743,7 +15743,7 @@
       </c>
       <c r="B766" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C766" t="n">
@@ -15751,7 +15751,7 @@
       </c>
       <c r="D766" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jun 22 04:05:59", "HOSTNAME": "combo", "PID": "16663", "USERNAME": "cyrus"}</t>
+          <t>{"TIMESTAMP": "Jun 22 04:05:59", "HOSTNAME": "combo", "PID": "16663", "STATE": "closed", "USERNAME": "cyrus"}</t>
         </is>
       </c>
     </row>
@@ -15763,7 +15763,7 @@
       </c>
       <c r="B767" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C767" t="n">
@@ -15771,7 +15771,7 @@
       </c>
       <c r="D767" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jun 22 04:11:42", "HOSTNAME": "combo", "PID": "17037", "USERNAME": "news"}</t>
+          <t>{"TIMESTAMP": "Jun 22 04:11:42", "HOSTNAME": "combo", "PID": "17037", "STATE": "closed", "USERNAME": "news"}</t>
         </is>
       </c>
     </row>
@@ -15783,7 +15783,7 @@
       </c>
       <c r="B768" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C768" t="n">
@@ -15791,7 +15791,7 @@
       </c>
       <c r="D768" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jun 21 04:06:58", "HOSTNAME": "combo", "PID": "12098", "USERNAME": "cyrus"}</t>
+          <t>{"TIMESTAMP": "Jun 21 04:06:58", "HOSTNAME": "combo", "PID": "12098", "STATE": "closed", "USERNAME": "cyrus"}</t>
         </is>
       </c>
     </row>
@@ -15803,7 +15803,7 @@
       </c>
       <c r="B769" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C769" t="n">
@@ -15811,7 +15811,7 @@
       </c>
       <c r="D769" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jun 21 04:13:04", "HOSTNAME": "combo", "PID": "13327", "USERNAME": "news"}</t>
+          <t>{"TIMESTAMP": "Jun 21 04:13:04", "HOSTNAME": "combo", "PID": "13327", "STATE": "closed", "USERNAME": "news"}</t>
         </is>
       </c>
     </row>
@@ -15823,7 +15823,7 @@
       </c>
       <c r="B770" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C770" t="n">
@@ -15831,7 +15831,7 @@
       </c>
       <c r="D770" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jun 20 04:02:54", "HOSTNAME": "combo", "PID": "9187", "USERNAME": "cyrus"}</t>
+          <t>{"TIMESTAMP": "Jun 20 04:02:54", "HOSTNAME": "combo", "PID": "9187", "STATE": "closed", "USERNAME": "cyrus"}</t>
         </is>
       </c>
     </row>
@@ -15843,7 +15843,7 @@
       </c>
       <c r="B771" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C771" t="n">
@@ -15851,7 +15851,7 @@
       </c>
       <c r="D771" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul 27 04:16:08", "HOSTNAME": "combo", "PID": "30999", "USERNAME": "cyrus"}</t>
+          <t>{"TIMESTAMP": "Jul 27 04:16:08", "HOSTNAME": "combo", "PID": "30999", "STATE": "closed", "USERNAME": "cyrus"}</t>
         </is>
       </c>
     </row>
@@ -15863,7 +15863,7 @@
       </c>
       <c r="B772" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C772" t="n">
@@ -15871,7 +15871,7 @@
       </c>
       <c r="D772" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul  2 04:04:02", "HOSTNAME": "combo", "PID": "24117", "USERNAME": "cyrus"}</t>
+          <t>{"TIMESTAMP": "Jul  2 04:04:02", "HOSTNAME": "combo", "PID": "24117", "STATE": "closed", "USERNAME": "cyrus"}</t>
         </is>
       </c>
     </row>
@@ -15883,7 +15883,7 @@
       </c>
       <c r="B773" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C773" t="n">
@@ -15891,7 +15891,7 @@
       </c>
       <c r="D773" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul  2 04:09:54", "HOSTNAME": "combo", "PID": "24511", "USERNAME": "news"}</t>
+          <t>{"TIMESTAMP": "Jul  2 04:09:54", "HOSTNAME": "combo", "PID": "24511", "STATE": "closed", "USERNAME": "news"}</t>
         </is>
       </c>
     </row>
@@ -15903,7 +15903,7 @@
       </c>
       <c r="B774" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C774" t="n">
@@ -15911,7 +15911,7 @@
       </c>
       <c r="D774" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul 26 04:05:23", "HOSTNAME": "combo", "PID": "27285", "USERNAME": "cyrus"}</t>
+          <t>{"TIMESTAMP": "Jul 26 04:05:23", "HOSTNAME": "combo", "PID": "27285", "STATE": "closed", "USERNAME": "cyrus"}</t>
         </is>
       </c>
     </row>
@@ -15923,7 +15923,7 @@
       </c>
       <c r="B775" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C775" t="n">
@@ -15931,7 +15931,7 @@
       </c>
       <c r="D775" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jun 16 04:10:23", "HOSTNAME": "combo", "PID": "25178", "USERNAME": "cyrus"}</t>
+          <t>{"TIMESTAMP": "Jun 16 04:10:23", "HOSTNAME": "combo", "PID": "25178", "STATE": "closed", "USERNAME": "cyrus"}</t>
         </is>
       </c>
     </row>
@@ -15943,7 +15943,7 @@
       </c>
       <c r="B776" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C776" t="n">
@@ -15951,7 +15951,7 @@
       </c>
       <c r="D776" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jun 16 04:16:18", "HOSTNAME": "combo", "PID": "25548", "USERNAME": "news"}</t>
+          <t>{"TIMESTAMP": "Jun 16 04:16:18", "HOSTNAME": "combo", "PID": "25548", "STATE": "closed", "USERNAME": "news"}</t>
         </is>
       </c>
     </row>
@@ -15963,7 +15963,7 @@
       </c>
       <c r="B777" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C777" t="n">
@@ -15971,7 +15971,7 @@
       </c>
       <c r="D777" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jun 17 04:03:34", "HOSTNAME": "combo", "PID": "27953", "USERNAME": "cyrus"}</t>
+          <t>{"TIMESTAMP": "Jun 17 04:03:34", "HOSTNAME": "combo", "PID": "27953", "STATE": "closed", "USERNAME": "cyrus"}</t>
         </is>
       </c>
     </row>
@@ -15983,7 +15983,7 @@
       </c>
       <c r="B778" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C778" t="n">
@@ -15991,7 +15991,7 @@
       </c>
       <c r="D778" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jun 17 04:09:45", "HOSTNAME": "combo", "PID": "29190", "USERNAME": "news"}</t>
+          <t>{"TIMESTAMP": "Jun 17 04:09:45", "HOSTNAME": "combo", "PID": "29190", "STATE": "closed", "USERNAME": "news"}</t>
         </is>
       </c>
     </row>
@@ -21843,7 +21843,7 @@
       </c>
       <c r="B1071" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C1071" t="n">
@@ -21851,7 +21851,7 @@
       </c>
       <c r="D1071" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul  7 07:18:12", "HOSTNAME": "combo", "PID": "12520", "USERNAME": "test", "UID": "509"}</t>
+          <t>{"TIMESTAMP": "Jul  7 07:18:12", "HOSTNAME": "combo", "PID": "12520", "STATE": "opened", "USERNAME": "test", "UID": "509"}</t>
         </is>
       </c>
     </row>
@@ -21863,7 +21863,7 @@
       </c>
       <c r="B1072" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C1072" t="n">
@@ -21871,7 +21871,7 @@
       </c>
       <c r="D1072" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul  1 05:02:27", "HOSTNAME": "combo", "PID": "21693", "USERNAME": "test", "UID": "509"}</t>
+          <t>{"TIMESTAMP": "Jul  1 05:02:27", "HOSTNAME": "combo", "PID": "21693", "STATE": "opened", "USERNAME": "test", "UID": "509"}</t>
         </is>
       </c>
     </row>
@@ -21883,7 +21883,7 @@
       </c>
       <c r="B1073" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C1073" t="n">
@@ -21891,7 +21891,7 @@
       </c>
       <c r="D1073" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jun 30 22:16:32", "HOSTNAME": "combo", "PID": "19433", "USERNAME": "test", "UID": "509"}</t>
+          <t>{"TIMESTAMP": "Jun 30 22:16:32", "HOSTNAME": "combo", "PID": "19433", "STATE": "opened", "USERNAME": "test", "UID": "509"}</t>
         </is>
       </c>
     </row>
@@ -21903,7 +21903,7 @@
       </c>
       <c r="B1074" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C1074" t="n">
@@ -21911,7 +21911,7 @@
       </c>
       <c r="D1074" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul  2 01:41:33", "HOSTNAME": "combo", "PID": "23545", "USERNAME": "test", "UID": "509"}</t>
+          <t>{"TIMESTAMP": "Jul  2 01:41:33", "HOSTNAME": "combo", "PID": "23545", "STATE": "opened", "USERNAME": "test", "UID": "509"}</t>
         </is>
       </c>
     </row>
@@ -21923,7 +21923,7 @@
       </c>
       <c r="B1075" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C1075" t="n">
@@ -21931,7 +21931,7 @@
       </c>
       <c r="D1075" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul  2 01:41:32", "HOSTNAME": "combo", "PID": "23536", "USERNAME": "test", "UID": "509"}</t>
+          <t>{"TIMESTAMP": "Jul  2 01:41:32", "HOSTNAME": "combo", "PID": "23536", "STATE": "opened", "USERNAME": "test", "UID": "509"}</t>
         </is>
       </c>
     </row>
@@ -21943,7 +21943,7 @@
       </c>
       <c r="B1076" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C1076" t="n">
@@ -21951,7 +21951,7 @@
       </c>
       <c r="D1076" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul  2 01:41:32", "HOSTNAME": "combo", "PID": "23534", "USERNAME": "test", "UID": "509"}</t>
+          <t>{"TIMESTAMP": "Jul  2 01:41:32", "HOSTNAME": "combo", "PID": "23534", "STATE": "opened", "USERNAME": "test", "UID": "509"}</t>
         </is>
       </c>
     </row>
@@ -21963,7 +21963,7 @@
       </c>
       <c r="B1077" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C1077" t="n">
@@ -21971,7 +21971,7 @@
       </c>
       <c r="D1077" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul  2 01:41:33", "HOSTNAME": "combo", "PID": "23546", "USERNAME": "test", "UID": "509"}</t>
+          <t>{"TIMESTAMP": "Jul  2 01:41:33", "HOSTNAME": "combo", "PID": "23546", "STATE": "opened", "USERNAME": "test", "UID": "509"}</t>
         </is>
       </c>
     </row>
@@ -21983,7 +21983,7 @@
       </c>
       <c r="B1078" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C1078" t="n">
@@ -21991,7 +21991,7 @@
       </c>
       <c r="D1078" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul  2 01:41:33", "HOSTNAME": "combo", "PID": "23547", "USERNAME": "test", "UID": "509"}</t>
+          <t>{"TIMESTAMP": "Jul  2 01:41:33", "HOSTNAME": "combo", "PID": "23547", "STATE": "opened", "USERNAME": "test", "UID": "509"}</t>
         </is>
       </c>
     </row>
@@ -22003,7 +22003,7 @@
       </c>
       <c r="B1079" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C1079" t="n">
@@ -22011,7 +22011,7 @@
       </c>
       <c r="D1079" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jun 30 22:16:32", "HOSTNAME": "combo", "PID": "19434", "USERNAME": "test", "UID": "509"}</t>
+          <t>{"TIMESTAMP": "Jun 30 22:16:32", "HOSTNAME": "combo", "PID": "19434", "STATE": "opened", "USERNAME": "test", "UID": "509"}</t>
         </is>
       </c>
     </row>
@@ -22023,7 +22023,7 @@
       </c>
       <c r="B1080" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C1080" t="n">
@@ -22031,7 +22031,7 @@
       </c>
       <c r="D1080" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul  1 05:02:26", "HOSTNAME": "combo", "PID": "21689", "USERNAME": "test", "UID": "509"}</t>
+          <t>{"TIMESTAMP": "Jul  1 05:02:26", "HOSTNAME": "combo", "PID": "21689", "STATE": "opened", "USERNAME": "test", "UID": "509"}</t>
         </is>
       </c>
     </row>
@@ -22043,7 +22043,7 @@
       </c>
       <c r="B1081" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C1081" t="n">
@@ -22051,7 +22051,7 @@
       </c>
       <c r="D1081" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jun 30 22:16:32", "HOSTNAME": "combo", "PID": "19435", "USERNAME": "test", "UID": "509"}</t>
+          <t>{"TIMESTAMP": "Jun 30 22:16:32", "HOSTNAME": "combo", "PID": "19435", "STATE": "opened", "USERNAME": "test", "UID": "509"}</t>
         </is>
       </c>
     </row>
@@ -22063,7 +22063,7 @@
       </c>
       <c r="B1082" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C1082" t="n">
@@ -22071,7 +22071,7 @@
       </c>
       <c r="D1082" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul  2 01:41:32", "HOSTNAME": "combo", "PID": "23535", "USERNAME": "test", "UID": "509"}</t>
+          <t>{"TIMESTAMP": "Jul  2 01:41:32", "HOSTNAME": "combo", "PID": "23535", "STATE": "opened", "USERNAME": "test", "UID": "509"}</t>
         </is>
       </c>
     </row>
@@ -22083,7 +22083,7 @@
       </c>
       <c r="B1083" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C1083" t="n">
@@ -22091,7 +22091,7 @@
       </c>
       <c r="D1083" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul 13 17:22:28", "HOSTNAME": "combo", "PID": "8113", "USERNAME": "test", "UID": "509"}</t>
+          <t>{"TIMESTAMP": "Jul 13 17:22:28", "HOSTNAME": "combo", "PID": "8113", "STATE": "opened", "USERNAME": "test", "UID": "509"}</t>
         </is>
       </c>
     </row>
@@ -22103,7 +22103,7 @@
       </c>
       <c r="B1084" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C1084" t="n">
@@ -22111,7 +22111,7 @@
       </c>
       <c r="D1084" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul 13 17:22:28", "HOSTNAME": "combo", "PID": "8114", "USERNAME": "test", "UID": "509"}</t>
+          <t>{"TIMESTAMP": "Jul 13 17:22:28", "HOSTNAME": "combo", "PID": "8114", "STATE": "opened", "USERNAME": "test", "UID": "509"}</t>
         </is>
       </c>
     </row>
@@ -22123,7 +22123,7 @@
       </c>
       <c r="B1085" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C1085" t="n">
@@ -22131,7 +22131,7 @@
       </c>
       <c r="D1085" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jun 17 20:29:26", "HOSTNAME": "combo", "PID": "30631", "USERNAME": "test", "UID": "509"}</t>
+          <t>{"TIMESTAMP": "Jun 17 20:29:26", "HOSTNAME": "combo", "PID": "30631", "STATE": "opened", "USERNAME": "test", "UID": "509"}</t>
         </is>
       </c>
     </row>
@@ -22143,7 +22143,7 @@
       </c>
       <c r="B1086" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C1086" t="n">
@@ -22151,7 +22151,7 @@
       </c>
       <c r="D1086" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul  1 09:14:43", "HOSTNAME": "combo", "PID": "22099", "USERNAME": "test", "UID": "509"}</t>
+          <t>{"TIMESTAMP": "Jul  1 09:14:43", "HOSTNAME": "combo", "PID": "22099", "STATE": "opened", "USERNAME": "test", "UID": "509"}</t>
         </is>
       </c>
     </row>
@@ -22163,7 +22163,7 @@
       </c>
       <c r="B1087" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C1087" t="n">
@@ -22171,7 +22171,7 @@
       </c>
       <c r="D1087" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul 13 17:22:29", "HOSTNAME": "combo", "PID": "8117", "USERNAME": "test", "UID": "509"}</t>
+          <t>{"TIMESTAMP": "Jul 13 17:22:29", "HOSTNAME": "combo", "PID": "8117", "STATE": "opened", "USERNAME": "test", "UID": "509"}</t>
         </is>
       </c>
     </row>
@@ -22183,7 +22183,7 @@
       </c>
       <c r="B1088" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C1088" t="n">
@@ -22191,7 +22191,7 @@
       </c>
       <c r="D1088" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul  1 05:02:26", "HOSTNAME": "combo", "PID": "21691", "USERNAME": "test", "UID": "509"}</t>
+          <t>{"TIMESTAMP": "Jul  1 05:02:26", "HOSTNAME": "combo", "PID": "21691", "STATE": "opened", "USERNAME": "test", "UID": "509"}</t>
         </is>
       </c>
     </row>
@@ -22203,7 +22203,7 @@
       </c>
       <c r="B1089" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C1089" t="n">
@@ -22211,7 +22211,7 @@
       </c>
       <c r="D1089" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul  1 09:14:43", "HOSTNAME": "combo", "PID": "22104", "USERNAME": "test", "UID": "509"}</t>
+          <t>{"TIMESTAMP": "Jul  1 09:14:43", "HOSTNAME": "combo", "PID": "22104", "STATE": "opened", "USERNAME": "test", "UID": "509"}</t>
         </is>
       </c>
     </row>
@@ -22223,7 +22223,7 @@
       </c>
       <c r="B1090" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C1090" t="n">
@@ -22231,7 +22231,7 @@
       </c>
       <c r="D1090" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul  7 07:18:12", "HOSTNAME": "combo", "PID": "12518", "USERNAME": "test", "UID": "509"}</t>
+          <t>{"TIMESTAMP": "Jul  7 07:18:12", "HOSTNAME": "combo", "PID": "12518", "STATE": "opened", "USERNAME": "test", "UID": "509"}</t>
         </is>
       </c>
     </row>
@@ -22243,7 +22243,7 @@
       </c>
       <c r="B1091" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C1091" t="n">
@@ -22251,7 +22251,7 @@
       </c>
       <c r="D1091" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul  7 07:18:12", "HOSTNAME": "combo", "PID": "12519", "USERNAME": "test", "UID": "509"}</t>
+          <t>{"TIMESTAMP": "Jul  7 07:18:12", "HOSTNAME": "combo", "PID": "12519", "STATE": "opened", "USERNAME": "test", "UID": "509"}</t>
         </is>
       </c>
     </row>
@@ -22263,7 +22263,7 @@
       </c>
       <c r="B1092" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C1092" t="n">
@@ -22271,7 +22271,7 @@
       </c>
       <c r="D1092" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul  1 09:14:43", "HOSTNAME": "combo", "PID": "22106", "USERNAME": "test", "UID": "509"}</t>
+          <t>{"TIMESTAMP": "Jul  1 09:14:43", "HOSTNAME": "combo", "PID": "22106", "STATE": "opened", "USERNAME": "test", "UID": "509"}</t>
         </is>
       </c>
     </row>
@@ -22283,7 +22283,7 @@
       </c>
       <c r="B1093" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C1093" t="n">
@@ -22291,7 +22291,7 @@
       </c>
       <c r="D1093" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul  1 05:02:26", "HOSTNAME": "combo", "PID": "21692", "USERNAME": "test", "UID": "509"}</t>
+          <t>{"TIMESTAMP": "Jul  1 05:02:26", "HOSTNAME": "combo", "PID": "21692", "STATE": "opened", "USERNAME": "test", "UID": "509"}</t>
         </is>
       </c>
     </row>
@@ -22303,7 +22303,7 @@
       </c>
       <c r="B1094" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C1094" t="n">
@@ -22311,7 +22311,7 @@
       </c>
       <c r="D1094" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jun 30 22:16:32", "HOSTNAME": "combo", "PID": "19439", "USERNAME": "test", "UID": "509"}</t>
+          <t>{"TIMESTAMP": "Jun 30 22:16:32", "HOSTNAME": "combo", "PID": "19439", "STATE": "opened", "USERNAME": "test", "UID": "509"}</t>
         </is>
       </c>
     </row>
@@ -22323,7 +22323,7 @@
       </c>
       <c r="B1095" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C1095" t="n">
@@ -22331,7 +22331,7 @@
       </c>
       <c r="D1095" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jun 30 22:16:32", "HOSTNAME": "combo", "PID": "19440", "USERNAME": "test", "UID": "509"}</t>
+          <t>{"TIMESTAMP": "Jun 30 22:16:32", "HOSTNAME": "combo", "PID": "19440", "STATE": "opened", "USERNAME": "test", "UID": "509"}</t>
         </is>
       </c>
     </row>
@@ -22343,7 +22343,7 @@
       </c>
       <c r="B1096" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C1096" t="n">
@@ -22351,7 +22351,7 @@
       </c>
       <c r="D1096" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul  2 01:41:32", "HOSTNAME": "combo", "PID": "23533", "USERNAME": "test", "UID": "509"}</t>
+          <t>{"TIMESTAMP": "Jul  2 01:41:32", "HOSTNAME": "combo", "PID": "23533", "STATE": "opened", "USERNAME": "test", "UID": "509"}</t>
         </is>
       </c>
     </row>
@@ -22363,7 +22363,7 @@
       </c>
       <c r="B1097" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C1097" t="n">
@@ -22371,7 +22371,7 @@
       </c>
       <c r="D1097" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul  7 07:18:13", "HOSTNAME": "combo", "PID": "12527", "USERNAME": "test", "UID": "509"}</t>
+          <t>{"TIMESTAMP": "Jul  7 07:18:13", "HOSTNAME": "combo", "PID": "12527", "STATE": "opened", "USERNAME": "test", "UID": "509"}</t>
         </is>
       </c>
     </row>
@@ -22383,7 +22383,7 @@
       </c>
       <c r="B1098" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C1098" t="n">
@@ -22391,7 +22391,7 @@
       </c>
       <c r="D1098" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jun 30 22:16:32", "HOSTNAME": "combo", "PID": "19437", "USERNAME": "test", "UID": "509"}</t>
+          <t>{"TIMESTAMP": "Jun 30 22:16:32", "HOSTNAME": "combo", "PID": "19437", "STATE": "opened", "USERNAME": "test", "UID": "509"}</t>
         </is>
       </c>
     </row>
@@ -22403,7 +22403,7 @@
       </c>
       <c r="B1099" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C1099" t="n">
@@ -22411,7 +22411,7 @@
       </c>
       <c r="D1099" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jun 30 22:16:32", "HOSTNAME": "combo", "PID": "19432", "USERNAME": "test", "UID": "509"}</t>
+          <t>{"TIMESTAMP": "Jun 30 22:16:32", "HOSTNAME": "combo", "PID": "19432", "STATE": "opened", "USERNAME": "test", "UID": "509"}</t>
         </is>
       </c>
     </row>
@@ -22423,7 +22423,7 @@
       </c>
       <c r="B1100" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C1100" t="n">
@@ -22431,7 +22431,7 @@
       </c>
       <c r="D1100" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul  7 07:18:13", "HOSTNAME": "combo", "PID": "12524", "USERNAME": "test", "UID": "509"}</t>
+          <t>{"TIMESTAMP": "Jul  7 07:18:13", "HOSTNAME": "combo", "PID": "12524", "STATE": "opened", "USERNAME": "test", "UID": "509"}</t>
         </is>
       </c>
     </row>
@@ -22443,7 +22443,7 @@
       </c>
       <c r="B1101" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C1101" t="n">
@@ -22451,7 +22451,7 @@
       </c>
       <c r="D1101" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul  7 07:18:13", "HOSTNAME": "combo", "PID": "12525", "USERNAME": "test", "UID": "509"}</t>
+          <t>{"TIMESTAMP": "Jul  7 07:18:13", "HOSTNAME": "combo", "PID": "12525", "STATE": "opened", "USERNAME": "test", "UID": "509"}</t>
         </is>
       </c>
     </row>
@@ -22463,7 +22463,7 @@
       </c>
       <c r="B1102" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C1102" t="n">
@@ -22471,7 +22471,7 @@
       </c>
       <c r="D1102" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul  2 01:41:33", "HOSTNAME": "combo", "PID": "23544", "USERNAME": "test", "UID": "509"}</t>
+          <t>{"TIMESTAMP": "Jul  2 01:41:33", "HOSTNAME": "combo", "PID": "23544", "STATE": "opened", "USERNAME": "test", "UID": "509"}</t>
         </is>
       </c>
     </row>
@@ -22483,7 +22483,7 @@
       </c>
       <c r="B1103" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C1103" t="n">
@@ -22491,7 +22491,7 @@
       </c>
       <c r="D1103" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul  1 09:14:44", "HOSTNAME": "combo", "PID": "22112", "USERNAME": "test", "UID": "509"}</t>
+          <t>{"TIMESTAMP": "Jul  1 09:14:44", "HOSTNAME": "combo", "PID": "22112", "STATE": "opened", "USERNAME": "test", "UID": "509"}</t>
         </is>
       </c>
     </row>
@@ -22503,7 +22503,7 @@
       </c>
       <c r="B1104" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C1104" t="n">
@@ -22511,7 +22511,7 @@
       </c>
       <c r="D1104" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jun 30 22:16:32", "HOSTNAME": "combo", "PID": "19431", "USERNAME": "test", "UID": "509"}</t>
+          <t>{"TIMESTAMP": "Jun 30 22:16:32", "HOSTNAME": "combo", "PID": "19431", "STATE": "opened", "USERNAME": "test", "UID": "509"}</t>
         </is>
       </c>
     </row>
@@ -22523,7 +22523,7 @@
       </c>
       <c r="B1105" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C1105" t="n">
@@ -22531,7 +22531,7 @@
       </c>
       <c r="D1105" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jun 30 22:16:32", "HOSTNAME": "combo", "PID": "19436", "USERNAME": "test", "UID": "509"}</t>
+          <t>{"TIMESTAMP": "Jun 30 22:16:32", "HOSTNAME": "combo", "PID": "19436", "STATE": "opened", "USERNAME": "test", "UID": "509"}</t>
         </is>
       </c>
     </row>
@@ -22543,7 +22543,7 @@
       </c>
       <c r="B1106" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C1106" t="n">
@@ -22551,7 +22551,7 @@
       </c>
       <c r="D1106" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jun 30 22:16:32", "HOSTNAME": "combo", "PID": "19438", "USERNAME": "test", "UID": "509"}</t>
+          <t>{"TIMESTAMP": "Jun 30 22:16:32", "HOSTNAME": "combo", "PID": "19438", "STATE": "opened", "USERNAME": "test", "UID": "509"}</t>
         </is>
       </c>
     </row>
@@ -22563,7 +22563,7 @@
       </c>
       <c r="B1107" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C1107" t="n">
@@ -22571,7 +22571,7 @@
       </c>
       <c r="D1107" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul  1 05:02:27", "HOSTNAME": "combo", "PID": "21693", "USERNAME": "test"}</t>
+          <t>{"TIMESTAMP": "Jul  1 05:02:27", "HOSTNAME": "combo", "PID": "21693", "STATE": "closed", "USERNAME": "test"}</t>
         </is>
       </c>
     </row>
@@ -22583,7 +22583,7 @@
       </c>
       <c r="B1108" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C1108" t="n">
@@ -22591,7 +22591,7 @@
       </c>
       <c r="D1108" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul  2 01:41:33", "HOSTNAME": "combo", "PID": "23545", "USERNAME": "test"}</t>
+          <t>{"TIMESTAMP": "Jul  2 01:41:33", "HOSTNAME": "combo", "PID": "23545", "STATE": "closed", "USERNAME": "test"}</t>
         </is>
       </c>
     </row>
@@ -22603,7 +22603,7 @@
       </c>
       <c r="B1109" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C1109" t="n">
@@ -22611,7 +22611,7 @@
       </c>
       <c r="D1109" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul  2 01:41:33", "HOSTNAME": "combo", "PID": "23547", "USERNAME": "test"}</t>
+          <t>{"TIMESTAMP": "Jul  2 01:41:33", "HOSTNAME": "combo", "PID": "23547", "STATE": "closed", "USERNAME": "test"}</t>
         </is>
       </c>
     </row>
@@ -22623,7 +22623,7 @@
       </c>
       <c r="B1110" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C1110" t="n">
@@ -22631,7 +22631,7 @@
       </c>
       <c r="D1110" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul 13 17:22:29", "HOSTNAME": "combo", "PID": "8113", "USERNAME": "test"}</t>
+          <t>{"TIMESTAMP": "Jul 13 17:22:29", "HOSTNAME": "combo", "PID": "8113", "STATE": "closed", "USERNAME": "test"}</t>
         </is>
       </c>
     </row>
@@ -22643,7 +22643,7 @@
       </c>
       <c r="B1111" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C1111" t="n">
@@ -22651,7 +22651,7 @@
       </c>
       <c r="D1111" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul 13 17:22:29", "HOSTNAME": "combo", "PID": "8114", "USERNAME": "test"}</t>
+          <t>{"TIMESTAMP": "Jul 13 17:22:29", "HOSTNAME": "combo", "PID": "8114", "STATE": "closed", "USERNAME": "test"}</t>
         </is>
       </c>
     </row>
@@ -22663,7 +22663,7 @@
       </c>
       <c r="B1112" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C1112" t="n">
@@ -22671,7 +22671,7 @@
       </c>
       <c r="D1112" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul 13 17:22:29", "HOSTNAME": "combo", "PID": "8117", "USERNAME": "test"}</t>
+          <t>{"TIMESTAMP": "Jul 13 17:22:29", "HOSTNAME": "combo", "PID": "8117", "STATE": "closed", "USERNAME": "test"}</t>
         </is>
       </c>
     </row>
@@ -22683,7 +22683,7 @@
       </c>
       <c r="B1113" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C1113" t="n">
@@ -22691,7 +22691,7 @@
       </c>
       <c r="D1113" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul  2 01:41:33", "HOSTNAME": "combo", "PID": "23546", "USERNAME": "test"}</t>
+          <t>{"TIMESTAMP": "Jul  2 01:41:33", "HOSTNAME": "combo", "PID": "23546", "STATE": "closed", "USERNAME": "test"}</t>
         </is>
       </c>
     </row>
@@ -22703,7 +22703,7 @@
       </c>
       <c r="B1114" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C1114" t="n">
@@ -22711,7 +22711,7 @@
       </c>
       <c r="D1114" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul  7 07:18:12", "HOSTNAME": "combo", "PID": "12518", "USERNAME": "test"}</t>
+          <t>{"TIMESTAMP": "Jul  7 07:18:12", "HOSTNAME": "combo", "PID": "12518", "STATE": "closed", "USERNAME": "test"}</t>
         </is>
       </c>
     </row>
@@ -22723,7 +22723,7 @@
       </c>
       <c r="B1115" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C1115" t="n">
@@ -22731,7 +22731,7 @@
       </c>
       <c r="D1115" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul  2 01:41:32", "HOSTNAME": "combo", "PID": "23535", "USERNAME": "test"}</t>
+          <t>{"TIMESTAMP": "Jul  2 01:41:32", "HOSTNAME": "combo", "PID": "23535", "STATE": "closed", "USERNAME": "test"}</t>
         </is>
       </c>
     </row>
@@ -22743,7 +22743,7 @@
       </c>
       <c r="B1116" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C1116" t="n">
@@ -22751,7 +22751,7 @@
       </c>
       <c r="D1116" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul  7 07:18:12", "HOSTNAME": "combo", "PID": "12520", "USERNAME": "test"}</t>
+          <t>{"TIMESTAMP": "Jul  7 07:18:12", "HOSTNAME": "combo", "PID": "12520", "STATE": "closed", "USERNAME": "test"}</t>
         </is>
       </c>
     </row>
@@ -22763,7 +22763,7 @@
       </c>
       <c r="B1117" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C1117" t="n">
@@ -22771,7 +22771,7 @@
       </c>
       <c r="D1117" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul  7 07:18:12", "HOSTNAME": "combo", "PID": "12519", "USERNAME": "test"}</t>
+          <t>{"TIMESTAMP": "Jul  7 07:18:12", "HOSTNAME": "combo", "PID": "12519", "STATE": "closed", "USERNAME": "test"}</t>
         </is>
       </c>
     </row>
@@ -22783,7 +22783,7 @@
       </c>
       <c r="B1118" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C1118" t="n">
@@ -22791,7 +22791,7 @@
       </c>
       <c r="D1118" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul  7 07:18:13", "HOSTNAME": "combo", "PID": "12524", "USERNAME": "test"}</t>
+          <t>{"TIMESTAMP": "Jul  7 07:18:13", "HOSTNAME": "combo", "PID": "12524", "STATE": "closed", "USERNAME": "test"}</t>
         </is>
       </c>
     </row>
@@ -22803,7 +22803,7 @@
       </c>
       <c r="B1119" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C1119" t="n">
@@ -22811,7 +22811,7 @@
       </c>
       <c r="D1119" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul  7 07:18:14", "HOSTNAME": "combo", "PID": "12527", "USERNAME": "test"}</t>
+          <t>{"TIMESTAMP": "Jul  7 07:18:14", "HOSTNAME": "combo", "PID": "12527", "STATE": "closed", "USERNAME": "test"}</t>
         </is>
       </c>
     </row>
@@ -22823,7 +22823,7 @@
       </c>
       <c r="B1120" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C1120" t="n">
@@ -22831,7 +22831,7 @@
       </c>
       <c r="D1120" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jun 30 22:16:33", "HOSTNAME": "combo", "PID": "19438", "USERNAME": "test"}</t>
+          <t>{"TIMESTAMP": "Jun 30 22:16:33", "HOSTNAME": "combo", "PID": "19438", "STATE": "closed", "USERNAME": "test"}</t>
         </is>
       </c>
     </row>
@@ -22843,7 +22843,7 @@
       </c>
       <c r="B1121" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C1121" t="n">
@@ -22851,7 +22851,7 @@
       </c>
       <c r="D1121" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jun 30 22:16:33", "HOSTNAME": "combo", "PID": "19439", "USERNAME": "test"}</t>
+          <t>{"TIMESTAMP": "Jun 30 22:16:33", "HOSTNAME": "combo", "PID": "19439", "STATE": "closed", "USERNAME": "test"}</t>
         </is>
       </c>
     </row>
@@ -22863,7 +22863,7 @@
       </c>
       <c r="B1122" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C1122" t="n">
@@ -22871,7 +22871,7 @@
       </c>
       <c r="D1122" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jun 30 22:16:33", "HOSTNAME": "combo", "PID": "19440", "USERNAME": "test"}</t>
+          <t>{"TIMESTAMP": "Jun 30 22:16:33", "HOSTNAME": "combo", "PID": "19440", "STATE": "closed", "USERNAME": "test"}</t>
         </is>
       </c>
     </row>
@@ -22883,7 +22883,7 @@
       </c>
       <c r="B1123" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C1123" t="n">
@@ -22891,7 +22891,7 @@
       </c>
       <c r="D1123" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jun 30 22:16:32", "HOSTNAME": "combo", "PID": "19434", "USERNAME": "test"}</t>
+          <t>{"TIMESTAMP": "Jun 30 22:16:32", "HOSTNAME": "combo", "PID": "19434", "STATE": "closed", "USERNAME": "test"}</t>
         </is>
       </c>
     </row>
@@ -22903,7 +22903,7 @@
       </c>
       <c r="B1124" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C1124" t="n">
@@ -22911,7 +22911,7 @@
       </c>
       <c r="D1124" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul  1 09:14:43", "HOSTNAME": "combo", "PID": "22104", "USERNAME": "test"}</t>
+          <t>{"TIMESTAMP": "Jul  1 09:14:43", "HOSTNAME": "combo", "PID": "22104", "STATE": "closed", "USERNAME": "test"}</t>
         </is>
       </c>
     </row>
@@ -22923,7 +22923,7 @@
       </c>
       <c r="B1125" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C1125" t="n">
@@ -22931,7 +22931,7 @@
       </c>
       <c r="D1125" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jun 30 22:16:32", "HOSTNAME": "combo", "PID": "19432", "USERNAME": "test"}</t>
+          <t>{"TIMESTAMP": "Jun 30 22:16:32", "HOSTNAME": "combo", "PID": "19432", "STATE": "closed", "USERNAME": "test"}</t>
         </is>
       </c>
     </row>
@@ -22943,7 +22943,7 @@
       </c>
       <c r="B1126" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C1126" t="n">
@@ -22951,7 +22951,7 @@
       </c>
       <c r="D1126" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul  1 05:02:26", "HOSTNAME": "combo", "PID": "21691", "USERNAME": "test"}</t>
+          <t>{"TIMESTAMP": "Jul  1 05:02:26", "HOSTNAME": "combo", "PID": "21691", "STATE": "closed", "USERNAME": "test"}</t>
         </is>
       </c>
     </row>
@@ -22963,7 +22963,7 @@
       </c>
       <c r="B1127" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C1127" t="n">
@@ -22971,7 +22971,7 @@
       </c>
       <c r="D1127" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jun 30 22:16:32", "HOSTNAME": "combo", "PID": "19431", "USERNAME": "test"}</t>
+          <t>{"TIMESTAMP": "Jun 30 22:16:32", "HOSTNAME": "combo", "PID": "19431", "STATE": "closed", "USERNAME": "test"}</t>
         </is>
       </c>
     </row>
@@ -22983,7 +22983,7 @@
       </c>
       <c r="B1128" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C1128" t="n">
@@ -22991,7 +22991,7 @@
       </c>
       <c r="D1128" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul  7 07:18:14", "HOSTNAME": "combo", "PID": "12525", "USERNAME": "test"}</t>
+          <t>{"TIMESTAMP": "Jul  7 07:18:14", "HOSTNAME": "combo", "PID": "12525", "STATE": "closed", "USERNAME": "test"}</t>
         </is>
       </c>
     </row>
@@ -23003,7 +23003,7 @@
       </c>
       <c r="B1129" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C1129" t="n">
@@ -23011,7 +23011,7 @@
       </c>
       <c r="D1129" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul  1 05:02:26", "HOSTNAME": "combo", "PID": "21689", "USERNAME": "test"}</t>
+          <t>{"TIMESTAMP": "Jul  1 05:02:26", "HOSTNAME": "combo", "PID": "21689", "STATE": "closed", "USERNAME": "test"}</t>
         </is>
       </c>
     </row>
@@ -23023,7 +23023,7 @@
       </c>
       <c r="B1130" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C1130" t="n">
@@ -23031,7 +23031,7 @@
       </c>
       <c r="D1130" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jun 30 22:16:33", "HOSTNAME": "combo", "PID": "19437", "USERNAME": "test"}</t>
+          <t>{"TIMESTAMP": "Jun 30 22:16:33", "HOSTNAME": "combo", "PID": "19437", "STATE": "closed", "USERNAME": "test"}</t>
         </is>
       </c>
     </row>
@@ -23043,7 +23043,7 @@
       </c>
       <c r="B1131" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C1131" t="n">
@@ -23051,7 +23051,7 @@
       </c>
       <c r="D1131" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jun 17 20:34:57", "HOSTNAME": "combo", "PID": "30631", "USERNAME": "test"}</t>
+          <t>{"TIMESTAMP": "Jun 17 20:34:57", "HOSTNAME": "combo", "PID": "30631", "STATE": "closed", "USERNAME": "test"}</t>
         </is>
       </c>
     </row>
@@ -23063,7 +23063,7 @@
       </c>
       <c r="B1132" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C1132" t="n">
@@ -23071,7 +23071,7 @@
       </c>
       <c r="D1132" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul  2 01:41:32", "HOSTNAME": "combo", "PID": "23533", "USERNAME": "test"}</t>
+          <t>{"TIMESTAMP": "Jul  2 01:41:32", "HOSTNAME": "combo", "PID": "23533", "STATE": "closed", "USERNAME": "test"}</t>
         </is>
       </c>
     </row>
@@ -23083,7 +23083,7 @@
       </c>
       <c r="B1133" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C1133" t="n">
@@ -23091,7 +23091,7 @@
       </c>
       <c r="D1133" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul  2 01:41:32", "HOSTNAME": "combo", "PID": "23534", "USERNAME": "test"}</t>
+          <t>{"TIMESTAMP": "Jul  2 01:41:32", "HOSTNAME": "combo", "PID": "23534", "STATE": "closed", "USERNAME": "test"}</t>
         </is>
       </c>
     </row>
@@ -23103,7 +23103,7 @@
       </c>
       <c r="B1134" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C1134" t="n">
@@ -23111,7 +23111,7 @@
       </c>
       <c r="D1134" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul  1 05:02:26", "HOSTNAME": "combo", "PID": "21692", "USERNAME": "test"}</t>
+          <t>{"TIMESTAMP": "Jul  1 05:02:26", "HOSTNAME": "combo", "PID": "21692", "STATE": "closed", "USERNAME": "test"}</t>
         </is>
       </c>
     </row>
@@ -23123,7 +23123,7 @@
       </c>
       <c r="B1135" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C1135" t="n">
@@ -23131,7 +23131,7 @@
       </c>
       <c r="D1135" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul  2 01:41:32", "HOSTNAME": "combo", "PID": "23536", "USERNAME": "test"}</t>
+          <t>{"TIMESTAMP": "Jul  2 01:41:32", "HOSTNAME": "combo", "PID": "23536", "STATE": "closed", "USERNAME": "test"}</t>
         </is>
       </c>
     </row>
@@ -23143,7 +23143,7 @@
       </c>
       <c r="B1136" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C1136" t="n">
@@ -23151,7 +23151,7 @@
       </c>
       <c r="D1136" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jun 30 22:16:32", "HOSTNAME": "combo", "PID": "19435", "USERNAME": "test"}</t>
+          <t>{"TIMESTAMP": "Jun 30 22:16:32", "HOSTNAME": "combo", "PID": "19435", "STATE": "closed", "USERNAME": "test"}</t>
         </is>
       </c>
     </row>
@@ -23163,7 +23163,7 @@
       </c>
       <c r="B1137" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C1137" t="n">
@@ -23171,7 +23171,7 @@
       </c>
       <c r="D1137" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul  2 01:41:33", "HOSTNAME": "combo", "PID": "23544", "USERNAME": "test"}</t>
+          <t>{"TIMESTAMP": "Jul  2 01:41:33", "HOSTNAME": "combo", "PID": "23544", "STATE": "closed", "USERNAME": "test"}</t>
         </is>
       </c>
     </row>
@@ -23183,7 +23183,7 @@
       </c>
       <c r="B1138" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C1138" t="n">
@@ -23191,7 +23191,7 @@
       </c>
       <c r="D1138" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul  1 09:14:44", "HOSTNAME": "combo", "PID": "22099", "USERNAME": "test"}</t>
+          <t>{"TIMESTAMP": "Jul  1 09:14:44", "HOSTNAME": "combo", "PID": "22099", "STATE": "closed", "USERNAME": "test"}</t>
         </is>
       </c>
     </row>
@@ -23203,7 +23203,7 @@
       </c>
       <c r="B1139" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C1139" t="n">
@@ -23211,7 +23211,7 @@
       </c>
       <c r="D1139" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jun 30 22:16:33", "HOSTNAME": "combo", "PID": "19433", "USERNAME": "test"}</t>
+          <t>{"TIMESTAMP": "Jun 30 22:16:33", "HOSTNAME": "combo", "PID": "19433", "STATE": "closed", "USERNAME": "test"}</t>
         </is>
       </c>
     </row>
@@ -23223,7 +23223,7 @@
       </c>
       <c r="B1140" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C1140" t="n">
@@ -23231,7 +23231,7 @@
       </c>
       <c r="D1140" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul  1 09:14:44", "HOSTNAME": "combo", "PID": "22106", "USERNAME": "test"}</t>
+          <t>{"TIMESTAMP": "Jul  1 09:14:44", "HOSTNAME": "combo", "PID": "22106", "STATE": "closed", "USERNAME": "test"}</t>
         </is>
       </c>
     </row>
@@ -23243,7 +23243,7 @@
       </c>
       <c r="B1141" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C1141" t="n">
@@ -23251,7 +23251,7 @@
       </c>
       <c r="D1141" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul  1 09:14:44", "HOSTNAME": "combo", "PID": "22112", "USERNAME": "test"}</t>
+          <t>{"TIMESTAMP": "Jul  1 09:14:44", "HOSTNAME": "combo", "PID": "22112", "STATE": "closed", "USERNAME": "test"}</t>
         </is>
       </c>
     </row>
@@ -23263,7 +23263,7 @@
       </c>
       <c r="B1142" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C1142" t="n">
@@ -23271,7 +23271,7 @@
       </c>
       <c r="D1142" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jun 30 22:16:33", "HOSTNAME": "combo", "PID": "19436", "USERNAME": "test"}</t>
+          <t>{"TIMESTAMP": "Jun 30 22:16:33", "HOSTNAME": "combo", "PID": "19436", "STATE": "closed", "USERNAME": "test"}</t>
         </is>
       </c>
     </row>
@@ -36583,7 +36583,7 @@
       </c>
       <c r="B1808" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; login(pam_unix)[&lt;PID&gt;]: session opened for user &lt;USERNAME&gt; by LOGIN(uid=&lt;UID&gt;)</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; login(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
         </is>
       </c>
       <c r="C1808" t="n">
@@ -36591,7 +36591,7 @@
       </c>
       <c r="D1808" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul  7 08:06:15", "HOSTNAME": "combo", "PID": "2421", "USERNAME": "root", "UID": "0"}</t>
+          <t>{"TIMESTAMP": "Jul  7 08:06:15", "HOSTNAME": "combo", "PID": "2421", "STATE": "opened", "USERNAME": "root", "UID": "0"}</t>
         </is>
       </c>
     </row>
@@ -36623,7 +36623,7 @@
       </c>
       <c r="B1810" t="inlineStr">
         <is>
-          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; login(pam_unix)[&lt;PID&gt;]: session closed for user &lt;USERNAME&gt;</t>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; login(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
         </is>
       </c>
       <c r="C1810" t="n">
@@ -36631,7 +36631,7 @@
       </c>
       <c r="D1810" t="inlineStr">
         <is>
-          <t>{"TIMESTAMP": "Jul  7 08:09:10", "HOSTNAME": "combo", "PID": "2421", "USERNAME": "root"}</t>
+          <t>{"TIMESTAMP": "Jul  7 08:09:10", "HOSTNAME": "combo", "PID": "2421", "STATE": "closed", "USERNAME": "root"}</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Template Freq Summary added
</commit_message>
<xml_diff>
--- a/Linux_2k_clean_analysis.xlsx
+++ b/Linux_2k_clean_analysis.xlsx
@@ -7,7 +7,8 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Log Analysis" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Template Summary" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -36858,4 +36859,339 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Template ID</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Template Pattern</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Occurrences</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>10</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; ftpd[&lt;PID&gt;]: connection from &lt;RHOST&gt;</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>3</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: authentication failure; logname= uid=&lt;UID&gt; euid=0 tty=NODEVssh ruser= rhost=&lt;RHOST&gt; user=&lt;USERNAME&gt;</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>6</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; ftpd[&lt;PID&gt;]: connection from &lt;RHOST&gt; (&lt;RHOST&gt;)</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>1</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: authentication failure; logname= uid=&lt;UID&gt; euid=0 tty=NODEVssh ruser= rhost=&lt;RHOST&gt;</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>2</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: check pass; user &lt;USERNAME&gt;</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>4</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; su(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; sshd(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>13</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; klogind[&lt;PID&gt;]: Kerberos authentication failed</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>14</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; klogind[&lt;PID&gt;]: Authentication failed from &lt;RHOST&gt; (&lt;RHOST&gt;): Software caused connection abort</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; klogind[&lt;PID&gt;]: Authentication failed from &lt;RHOST&gt; (&lt;RHOST&gt;): Permission denied in replay cache code</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>22</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; ftpd[&lt;PID&gt;]: getpeername (ftpd): Transport endpoint is not connected</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>21</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; ftpd[&lt;PID&gt;]: ANONYMOUS FTP LOGIN FROM &lt;RHOST&gt;</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>23</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; xinetd[&lt;PID&gt;]: warning: can't get client address: Connection reset by peer</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; login(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt; by (uid=&lt;UID&gt;)</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>11</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; snmpd[&lt;PID&gt;]: Received SNMP packet(s) from &lt;RHOST&gt;</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>9</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; ftpd[&lt;PID&gt;]: User unknown timed out after &lt;NUM&gt; seconds</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>16</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; -- root[&lt;PID&gt;]: ROOT LOGIN ON tty2</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; gdm(pam_unix)[&lt;PID&gt;]: authentication failure; logname= uid=&lt;UID&gt; euid=0 tty=:0 ruser= rhost=</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>18</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; gdm(pam_unix)[&lt;PID&gt;]: check pass; user &lt;USERNAME&gt;</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>17</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; login(pam_unix)[&lt;PID&gt;]: session &lt;STATE&gt; for user &lt;USERNAME&gt;</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>20</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>&lt;TIMESTAMP&gt; &lt;HOSTNAME&gt; gdm-binary[&lt;PID&gt;]: Couldn't authenticate user</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>